<commit_message>
updated belfb for upcoming q4
</commit_message>
<xml_diff>
--- a/BELFB.xlsx
+++ b/BELFB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/jgarza25_illinois_edu/Documents/Stock Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobgarza/repos/Stock_Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="573" documentId="11_C8706DE7DCCB40836B02CE998F75CCDC64E19E90" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A18260A-76CC-41F2-8EE6-D69EA7BC2BC9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2C7E62-2BEC-0D47-BDBA-4512C33372BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="795" windowWidth="28440" windowHeight="18615" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11220" yWindow="500" windowWidth="28040" windowHeight="15060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -247,10 +247,10 @@
     <t>MS Y/Y</t>
   </si>
   <si>
-    <t>Q323*</t>
+    <t>P/L</t>
   </si>
   <si>
-    <t>P/L</t>
+    <t>Q323</t>
   </si>
 </sst>
 </file>
@@ -261,7 +261,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,12 +284,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -480,7 +474,7 @@
                   <c:v>Q223</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Q323*</c:v>
+                  <c:v>Q323</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -543,7 +537,7 @@
                   <c:v>87.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>78.39</c:v>
+                  <c:v>74.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -635,7 +629,7 @@
                   <c:v>Q223</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Q323*</c:v>
+                  <c:v>Q323</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -698,7 +692,7 @@
                   <c:v>54.8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>54.8</c:v>
+                  <c:v>51.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,7 +784,7 @@
                   <c:v>Q223</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Q323*</c:v>
+                  <c:v>Q323</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -853,7 +847,7 @@
                   <c:v>26.8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28.14</c:v>
+                  <c:v>32.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1195,7 +1189,7 @@
                   <c:v>Q223</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Q323*</c:v>
+                  <c:v>Q323</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1261,7 +1255,7 @@
                   <c:v>87.1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>78.39</c:v>
+                  <c:v>74.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1356,7 +1350,7 @@
                   <c:v>Q223</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Q323*</c:v>
+                  <c:v>Q323</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1422,7 +1416,7 @@
                   <c:v>54.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>54.8</c:v>
+                  <c:v>51.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1511,7 @@
                   <c:v>Q223</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Q323*</c:v>
+                  <c:v>Q323</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1583,7 +1577,7 @@
                   <c:v>26.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28.14</c:v>
+                  <c:v>32.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2882,16 +2876,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>804863</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>17462</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>26194</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>140494</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2905,9 +2899,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="17342644" y="26194"/>
-          <a:ext cx="50006" cy="8305800"/>
+        <a:xfrm>
+          <a:off x="20750212" y="0"/>
+          <a:ext cx="14288" cy="8286750"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2983,15 +2977,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>708420</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>98822</xdr:rowOff>
+      <xdr:colOff>279795</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146447</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>619123</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>178594</xdr:rowOff>
+      <xdr:colOff>190498</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3019,14 +3013,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>738195</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:colOff>468320</xdr:colOff>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>142883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>750094</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:colOff>480219</xdr:colOff>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>154781</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3359,16 +3353,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -3376,11 +3370,10 @@
         <v>6</v>
       </c>
       <c r="K1" s="5">
-        <v>52.6</v>
+        <v>73.91</v>
       </c>
       <c r="L1" s="5">
-        <f>48.6</f>
-        <v>48.6</v>
+        <v>76.66</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -3389,7 +3382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J2" t="s">
         <v>5</v>
       </c>
@@ -3397,7 +3390,7 @@
         <v>10.632</v>
       </c>
       <c r="L2" s="5">
-        <v>2.1</v>
+        <v>2.14</v>
       </c>
       <c r="M2" t="s">
         <v>12</v>
@@ -3406,40 +3399,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J3" t="s">
         <v>7</v>
       </c>
       <c r="K3" s="5">
         <f>K1*K2</f>
-        <v>559.2432</v>
+        <v>785.81111999999996</v>
       </c>
       <c r="L3" s="5">
         <f>L1*L2</f>
-        <v>102.06</v>
+        <v>164.05240000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J4" t="s">
         <v>7</v>
       </c>
       <c r="K4" s="5">
         <f>K3+L3</f>
-        <v>661.30320000000006</v>
+        <v>949.86351999999999</v>
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J5" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="5">
-        <f>108.96</f>
-        <v>108.96</v>
+        <v>100.2</v>
       </c>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J6" t="s">
         <v>9</v>
       </c>
@@ -3448,27 +3440,27 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J7" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="5">
         <f>K4-K5+K6</f>
-        <v>612.34320000000002</v>
+        <v>909.66351999999995</v>
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>57</v>
       </c>
@@ -3488,19 +3480,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3515,20 +3507,20 @@
   <dimension ref="A1:OX37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
+      <selection pane="bottomRight" activeCell="AB34" sqref="AB34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -3588,7 +3580,7 @@
         <v>32</v>
       </c>
       <c r="U1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="V1" t="s">
         <v>33</v>
@@ -3650,7 +3642,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>58</v>
@@ -3710,11 +3702,10 @@
         <v>87.1</v>
       </c>
       <c r="U2">
-        <f>T2*0.9</f>
-        <v>78.39</v>
+        <v>74.8</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
         <v>56</v>
@@ -3774,10 +3765,10 @@
         <v>54.8</v>
       </c>
       <c r="U3">
-        <v>54.8</v>
+        <v>51.7</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
         <v>57</v>
@@ -3837,16 +3828,15 @@
         <v>26.8</v>
       </c>
       <c r="U4">
-        <f>26.8*1.05</f>
-        <v>28.14</v>
+        <v>32.04</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3867,7 +3857,7 @@
       <c r="S6" s="5"/>
       <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -3927,7 +3917,7 @@
       </c>
       <c r="U7" s="5">
         <f>SUM(U2:U4)</f>
-        <v>161.32999999999998</v>
+        <v>158.54</v>
       </c>
       <c r="V7" s="5">
         <v>152</v>
@@ -3949,51 +3939,51 @@
         <v>654.21</v>
       </c>
       <c r="AB7" s="9">
-        <f>AA7*1</f>
-        <v>654.21</v>
+        <f>SUM(S7:V7)</f>
+        <v>651.65</v>
       </c>
       <c r="AC7" s="9">
         <f>AB7*1.03</f>
-        <v>673.83630000000005</v>
+        <v>671.19949999999994</v>
       </c>
       <c r="AD7" s="9">
         <f t="shared" ref="AD7:AL7" si="1">AC7*1.03</f>
-        <v>694.05138900000009</v>
+        <v>691.33548499999995</v>
       </c>
       <c r="AE7" s="9">
         <f t="shared" si="1"/>
-        <v>714.87293067000007</v>
+        <v>712.07554955000001</v>
       </c>
       <c r="AF7" s="9">
         <f t="shared" si="1"/>
-        <v>736.31911859010006</v>
+        <v>733.43781603650007</v>
       </c>
       <c r="AG7" s="9">
         <f t="shared" si="1"/>
-        <v>758.40869214780309</v>
+        <v>755.44095051759507</v>
       </c>
       <c r="AH7" s="9">
         <f t="shared" si="1"/>
-        <v>781.16095291223724</v>
+        <v>778.10417903312293</v>
       </c>
       <c r="AI7" s="9">
         <f t="shared" si="1"/>
-        <v>804.59578149960441</v>
+        <v>801.44730440411661</v>
       </c>
       <c r="AJ7" s="9">
         <f t="shared" si="1"/>
-        <v>828.73365494459256</v>
+        <v>825.49072353624013</v>
       </c>
       <c r="AK7" s="9">
         <f t="shared" si="1"/>
-        <v>853.59566459293035</v>
+        <v>850.25544524232737</v>
       </c>
       <c r="AL7" s="9">
         <f t="shared" si="1"/>
-        <v>879.20353453071823</v>
+        <v>875.76310859959722</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>35</v>
       </c>
@@ -4051,7 +4041,9 @@
       <c r="T8" s="5">
         <v>113.24</v>
       </c>
-      <c r="U8" s="5"/>
+      <c r="U8" s="5">
+        <v>103.2</v>
+      </c>
       <c r="X8" s="5">
         <f>SUM(C8:F8)</f>
         <v>381.88</v>
@@ -4069,7 +4061,7 @@
         <v>470.6</v>
       </c>
     </row>
-    <row r="9" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>36</v>
       </c>
@@ -4145,7 +4137,10 @@
         <f t="shared" si="2"/>
         <v>55.530000000000015</v>
       </c>
-      <c r="U9" s="7"/>
+      <c r="U9" s="7">
+        <f t="shared" ref="U9" si="3">U7-U8</f>
+        <v>55.339999999999989</v>
+      </c>
       <c r="X9" s="7">
         <f>X7-X8</f>
         <v>110.5</v>
@@ -4164,50 +4159,50 @@
       </c>
       <c r="AB9" s="10">
         <f>AB7*0.33</f>
-        <v>215.88930000000002</v>
+        <v>215.0445</v>
       </c>
       <c r="AC9" s="10">
-        <f t="shared" ref="AC9:AL9" si="3">AC7*0.33</f>
-        <v>222.36597900000004</v>
+        <f t="shared" ref="AC9:AL9" si="4">AC7*0.33</f>
+        <v>221.495835</v>
       </c>
       <c r="AD9" s="10">
-        <f t="shared" si="3"/>
-        <v>229.03695837000004</v>
+        <f t="shared" si="4"/>
+        <v>228.14071005</v>
       </c>
       <c r="AE9" s="10">
-        <f t="shared" si="3"/>
-        <v>235.90806712110003</v>
+        <f t="shared" si="4"/>
+        <v>234.98493135150002</v>
       </c>
       <c r="AF9" s="10">
-        <f t="shared" si="3"/>
-        <v>242.98530913473303</v>
+        <f t="shared" si="4"/>
+        <v>242.03447929204503</v>
       </c>
       <c r="AG9" s="10">
-        <f t="shared" si="3"/>
-        <v>250.27486840877503</v>
+        <f t="shared" si="4"/>
+        <v>249.29551367080637</v>
       </c>
       <c r="AH9" s="10">
-        <f t="shared" si="3"/>
-        <v>257.78311446103828</v>
+        <f t="shared" si="4"/>
+        <v>256.7743790809306</v>
       </c>
       <c r="AI9" s="10">
-        <f t="shared" si="3"/>
-        <v>265.51660789486948</v>
+        <f t="shared" si="4"/>
+        <v>264.47761045335847</v>
       </c>
       <c r="AJ9" s="10">
-        <f t="shared" si="3"/>
-        <v>273.48210613171557</v>
+        <f t="shared" si="4"/>
+        <v>272.41193876695928</v>
       </c>
       <c r="AK9" s="10">
-        <f t="shared" si="3"/>
-        <v>281.68656931566704</v>
+        <f t="shared" si="4"/>
+        <v>280.58429692996805</v>
       </c>
       <c r="AL9" s="10">
-        <f t="shared" si="3"/>
-        <v>290.13716639513706</v>
+        <f t="shared" si="4"/>
+        <v>289.0018258378671</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>37</v>
       </c>
@@ -4265,25 +4260,27 @@
       <c r="T10" s="5">
         <v>6</v>
       </c>
-      <c r="U10" s="5"/>
+      <c r="U10" s="5">
+        <v>5.29</v>
+      </c>
       <c r="X10" s="5">
         <f>SUM(C10:F10)</f>
         <v>26.9</v>
       </c>
       <c r="Y10" s="5">
-        <f t="shared" ref="Y10:Y11" si="4">SUM(G10:J10)</f>
+        <f t="shared" ref="Y10:Y11" si="5">SUM(G10:J10)</f>
         <v>23.56</v>
       </c>
       <c r="Z10" s="5">
-        <f t="shared" ref="Z10:Z16" si="5">SUM(K10:N10)</f>
+        <f t="shared" ref="Z10:Z16" si="6">SUM(K10:N10)</f>
         <v>21.94</v>
       </c>
       <c r="AA10" s="5">
-        <f t="shared" ref="AA10:AA11" si="6">SUM(O10:R10)</f>
+        <f t="shared" ref="AA10:AA11" si="7">SUM(O10:R10)</f>
         <v>20.380000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -4341,101 +4338,106 @@
       <c r="T11" s="5">
         <v>25.13</v>
       </c>
-      <c r="U11" s="5"/>
+      <c r="U11" s="5">
+        <v>23.7</v>
+      </c>
       <c r="X11" s="5">
         <f>SUM(C11:F11)</f>
         <v>76.5</v>
       </c>
       <c r="Y11" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78.515000000000001</v>
       </c>
       <c r="Z11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>85.84</v>
       </c>
       <c r="AA11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>92.320000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" ref="C12:T12" si="7">C10+C11</f>
+        <f t="shared" ref="C12:T12" si="8">C10+C11</f>
         <v>26.4</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26.06</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24.66</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26.279999999999998</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.11</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24.11</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24.59</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25.265000000000001</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25.97</v>
       </c>
       <c r="L12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27.28</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27.09</v>
       </c>
       <c r="N12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27.44</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26.02</v>
       </c>
       <c r="P12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.62</v>
       </c>
       <c r="Q12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27.09</v>
       </c>
       <c r="R12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>30.97</v>
       </c>
       <c r="S12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>30.509999999999998</v>
       </c>
       <c r="T12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>31.13</v>
       </c>
-      <c r="U12" s="5"/>
+      <c r="U12" s="5">
+        <f t="shared" ref="U12" si="9">U10+U11</f>
+        <v>28.99</v>
+      </c>
       <c r="X12" s="5">
         <f>X10+X11</f>
         <v>103.4</v>
@@ -4453,83 +4455,86 @@
         <v>112.70000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" ref="C13:T13" si="8">C9-C12</f>
+        <f t="shared" ref="C13:T13" si="10">C9-C12</f>
         <v>4.3399999999999963</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.75000000000000355</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.9499999999999993</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1.9399999999999942</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.9899999999999949</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7.6599999999999966</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8.9499999999999922</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1149999999999949</v>
       </c>
       <c r="K13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1.6999999999999886</v>
       </c>
       <c r="L13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.9300000000000068</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8.8800000000000132</v>
       </c>
       <c r="N13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>11.829999999999981</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8.100000000000005</v>
       </c>
       <c r="P13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>16.829999999999988</v>
       </c>
       <c r="Q13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>24.439999999999987</v>
       </c>
       <c r="R13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.539999999999992</v>
       </c>
       <c r="S13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>23.15</v>
       </c>
       <c r="T13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>24.400000000000016</v>
       </c>
-      <c r="U13" s="5"/>
+      <c r="U13" s="5">
+        <f t="shared" ref="U13" si="11">U9-U12</f>
+        <v>26.349999999999991</v>
+      </c>
       <c r="X13" s="5">
         <f>X9-X12</f>
         <v>7.0999999999999943</v>
@@ -4547,7 +4552,7 @@
         <v>70.91</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>45</v>
       </c>
@@ -4606,101 +4611,106 @@
       <c r="T14" s="5">
         <v>0.9</v>
       </c>
-      <c r="U14" s="5"/>
+      <c r="U14" s="5">
+        <v>-0.1</v>
+      </c>
       <c r="X14" s="5">
         <f>SUM(C14:F14)</f>
         <v>5.36</v>
       </c>
       <c r="Y14" s="5">
-        <f t="shared" ref="Y14:Y16" si="9">SUM(G14:J14)</f>
+        <f t="shared" ref="Y14:Y16" si="12">SUM(G14:J14)</f>
         <v>4.74</v>
       </c>
       <c r="Z14" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.53</v>
       </c>
       <c r="AA14" s="5">
-        <f t="shared" ref="AA14:AA16" si="10">SUM(O14:R14)</f>
+        <f t="shared" ref="AA14:AA16" si="13">SUM(O14:R14)</f>
         <v>3.35</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" ref="C15:T15" si="11">C13-C14</f>
+        <f t="shared" ref="C15:T15" si="14">C13-C14</f>
         <v>2.8999999999999964</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-0.54999999999999649</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>2.6499999999999995</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-3.2599999999999945</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-4.3399999999999945</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>6.4099999999999966</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>7.709999999999992</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>3.214999999999995</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-2.4999999999999885</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>6.2100000000000071</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>7.390000000000013</v>
       </c>
       <c r="N15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>11.309999999999981</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>7.4200000000000053</v>
       </c>
       <c r="P15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>16.059999999999988</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>23.499999999999986</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>20.579999999999991</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>22.169999999999998</v>
       </c>
       <c r="T15" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>23.500000000000018</v>
       </c>
-      <c r="U15" s="5"/>
+      <c r="U15" s="5">
+        <f t="shared" ref="U15" si="15">U13-U14</f>
+        <v>26.449999999999992</v>
+      </c>
       <c r="X15" s="5">
         <f>X13-X14</f>
         <v>1.739999999999994</v>
@@ -4718,7 +4728,7 @@
         <v>67.56</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>42</v>
       </c>
@@ -4776,25 +4786,27 @@
       <c r="T16" s="5">
         <v>-0.47</v>
       </c>
-      <c r="U16" s="5"/>
+      <c r="U16" s="5">
+        <v>4.3</v>
+      </c>
       <c r="X16" s="5">
         <f>SUM(C16:F16)</f>
         <v>1.4300000000000002</v>
       </c>
       <c r="Y16" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-0.60699999999999998</v>
       </c>
       <c r="Z16" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.4899999999999998</v>
       </c>
       <c r="AA16" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>6.41</v>
       </c>
     </row>
-    <row r="17" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>43</v>
       </c>
@@ -4803,51 +4815,51 @@
         <v>2.8699999999999966</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" ref="C17:O17" si="12">D15-D16</f>
+        <f t="shared" ref="D17:O17" si="16">D15-D16</f>
         <v>-0.96999999999999642</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>2.0599999999999996</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.6499999999999946</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.6199999999999948</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>5.9869999999999965</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.789999999999992</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>2.444999999999995</v>
       </c>
       <c r="K17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.4899999999999887</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.0600000000000076</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>5.9500000000000135</v>
       </c>
       <c r="N17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>9.3999999999999808</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>5.8600000000000048</v>
       </c>
       <c r="P17" s="5">
@@ -4870,8 +4882,8 @@
         <v>23.970000000000017</v>
       </c>
       <c r="U17" s="5">
-        <f>U7*0.14</f>
-        <v>22.586200000000002</v>
+        <f>U15-U16</f>
+        <v>22.149999999999991</v>
       </c>
       <c r="V17" s="5">
         <f>V7*0.14</f>
@@ -4895,1554 +4907,1554 @@
       </c>
       <c r="AB17" s="5">
         <f>AB7*0.13</f>
-        <v>85.047300000000007</v>
+        <v>84.714500000000001</v>
       </c>
       <c r="AC17" s="5">
         <f>AC7*0.14</f>
-        <v>94.337082000000009</v>
+        <v>93.967929999999996</v>
       </c>
       <c r="AD17" s="5">
-        <f t="shared" ref="AD17:AL17" si="13">AD7*0.14</f>
-        <v>97.167194460000019</v>
+        <f t="shared" ref="AD17:AL17" si="17">AD7*0.14</f>
+        <v>96.786967900000008</v>
       </c>
       <c r="AE17" s="5">
-        <f t="shared" si="13"/>
-        <v>100.08221029380002</v>
+        <f t="shared" si="17"/>
+        <v>99.690576937000017</v>
       </c>
       <c r="AF17" s="5">
-        <f t="shared" si="13"/>
-        <v>103.08467660261402</v>
+        <f t="shared" si="17"/>
+        <v>102.68129424511002</v>
       </c>
       <c r="AG17" s="5">
-        <f t="shared" si="13"/>
-        <v>106.17721690069244</v>
+        <f t="shared" si="17"/>
+        <v>105.76173307246331</v>
       </c>
       <c r="AH17" s="5">
-        <f t="shared" si="13"/>
-        <v>109.36253340771323</v>
+        <f t="shared" si="17"/>
+        <v>108.93458506463722</v>
       </c>
       <c r="AI17" s="5">
-        <f t="shared" si="13"/>
-        <v>112.64340940994462</v>
+        <f t="shared" si="17"/>
+        <v>112.20262261657633</v>
       </c>
       <c r="AJ17" s="5">
-        <f t="shared" si="13"/>
-        <v>116.02271169224296</v>
+        <f t="shared" si="17"/>
+        <v>115.56870129507362</v>
       </c>
       <c r="AK17" s="5">
-        <f t="shared" si="13"/>
-        <v>119.50339304301026</v>
+        <f t="shared" si="17"/>
+        <v>119.03576233392585</v>
       </c>
       <c r="AL17" s="5">
-        <f t="shared" si="13"/>
-        <v>123.08849483430056</v>
+        <f t="shared" si="17"/>
+        <v>122.60683520394362</v>
       </c>
       <c r="AM17" s="5">
         <f>AL17*(1+$AQ$30)</f>
-        <v>121.85760988595756</v>
+        <v>121.38076685190418</v>
       </c>
       <c r="AN17" s="5">
-        <f t="shared" ref="AN17:CY17" si="14">AM17*(1+$AQ$30)</f>
-        <v>120.63903378709799</v>
+        <f t="shared" ref="AN17:CY17" si="18">AM17*(1+$AQ$30)</f>
+        <v>120.16695918338515</v>
       </c>
       <c r="AO17" s="5">
-        <f t="shared" si="14"/>
-        <v>119.432643449227</v>
+        <f t="shared" si="18"/>
+        <v>118.9652895915513</v>
       </c>
       <c r="AP17" s="5">
-        <f t="shared" si="14"/>
-        <v>118.23831701473473</v>
+        <f t="shared" si="18"/>
+        <v>117.77563669563578</v>
       </c>
       <c r="AQ17" s="5">
-        <f t="shared" si="14"/>
-        <v>117.05593384458739</v>
+        <f t="shared" si="18"/>
+        <v>116.59788032867942</v>
       </c>
       <c r="AR17" s="5">
-        <f t="shared" si="14"/>
-        <v>115.88537450614152</v>
+        <f t="shared" si="18"/>
+        <v>115.43190152539263</v>
       </c>
       <c r="AS17" s="5">
-        <f t="shared" si="14"/>
-        <v>114.7265207610801</v>
+        <f t="shared" si="18"/>
+        <v>114.2775825101387</v>
       </c>
       <c r="AT17" s="5">
-        <f t="shared" si="14"/>
-        <v>113.5792555534693</v>
+        <f t="shared" si="18"/>
+        <v>113.13480668503732</v>
       </c>
       <c r="AU17" s="5">
-        <f t="shared" si="14"/>
-        <v>112.4434629979346</v>
+        <f t="shared" si="18"/>
+        <v>112.00345861818694</v>
       </c>
       <c r="AV17" s="5">
-        <f t="shared" si="14"/>
-        <v>111.31902836795526</v>
+        <f t="shared" si="18"/>
+        <v>110.88342403200507</v>
       </c>
       <c r="AW17" s="5">
-        <f t="shared" si="14"/>
-        <v>110.2058380842757</v>
+        <f t="shared" si="18"/>
+        <v>109.77458979168502</v>
       </c>
       <c r="AX17" s="5">
-        <f t="shared" si="14"/>
-        <v>109.10377970343293</v>
+        <f t="shared" si="18"/>
+        <v>108.67684389376817</v>
       </c>
       <c r="AY17" s="5">
-        <f t="shared" si="14"/>
-        <v>108.0127419063986</v>
+        <f t="shared" si="18"/>
+        <v>107.59007545483048</v>
       </c>
       <c r="AZ17" s="5">
-        <f t="shared" si="14"/>
-        <v>106.93261448733462</v>
+        <f t="shared" si="18"/>
+        <v>106.51417470028218</v>
       </c>
       <c r="BA17" s="5">
-        <f t="shared" si="14"/>
-        <v>105.86328834246127</v>
+        <f t="shared" si="18"/>
+        <v>105.44903295327936</v>
       </c>
       <c r="BB17" s="5">
-        <f t="shared" si="14"/>
-        <v>104.80465545903667</v>
+        <f t="shared" si="18"/>
+        <v>104.39454262374656</v>
       </c>
       <c r="BC17" s="5">
-        <f t="shared" si="14"/>
-        <v>103.7566089044463</v>
+        <f t="shared" si="18"/>
+        <v>103.35059719750909</v>
       </c>
       <c r="BD17" s="5">
-        <f t="shared" si="14"/>
-        <v>102.71904281540183</v>
+        <f t="shared" si="18"/>
+        <v>102.317091225534</v>
       </c>
       <c r="BE17" s="5">
-        <f t="shared" si="14"/>
-        <v>101.69185238724782</v>
+        <f t="shared" si="18"/>
+        <v>101.29392031327866</v>
       </c>
       <c r="BF17" s="5">
-        <f t="shared" si="14"/>
-        <v>100.67493386337534</v>
+        <f t="shared" si="18"/>
+        <v>100.28098111014587</v>
       </c>
       <c r="BG17" s="5">
-        <f t="shared" si="14"/>
-        <v>99.668184524741591</v>
+        <f t="shared" si="18"/>
+        <v>99.278171299044416</v>
       </c>
       <c r="BH17" s="5">
-        <f t="shared" si="14"/>
-        <v>98.671502679494168</v>
+        <f t="shared" si="18"/>
+        <v>98.285389586053967</v>
       </c>
       <c r="BI17" s="5">
-        <f t="shared" si="14"/>
-        <v>97.684787652699228</v>
+        <f t="shared" si="18"/>
+        <v>97.302535690193423</v>
       </c>
       <c r="BJ17" s="5">
-        <f t="shared" si="14"/>
-        <v>96.707939776172239</v>
+        <f t="shared" si="18"/>
+        <v>96.329510333291495</v>
       </c>
       <c r="BK17" s="5">
-        <f t="shared" si="14"/>
-        <v>95.740860378410517</v>
+        <f t="shared" si="18"/>
+        <v>95.366215229958584</v>
       </c>
       <c r="BL17" s="5">
-        <f t="shared" si="14"/>
-        <v>94.783451774626414</v>
+        <f t="shared" si="18"/>
+        <v>94.412553077658998</v>
       </c>
       <c r="BM17" s="5">
-        <f t="shared" si="14"/>
-        <v>93.835617256880155</v>
+        <f t="shared" si="18"/>
+        <v>93.46842754688241</v>
       </c>
       <c r="BN17" s="5">
-        <f t="shared" si="14"/>
-        <v>92.897261084311353</v>
+        <f t="shared" si="18"/>
+        <v>92.533743271413584</v>
       </c>
       <c r="BO17" s="5">
-        <f t="shared" si="14"/>
-        <v>91.968288473468235</v>
+        <f t="shared" si="18"/>
+        <v>91.608405838699454</v>
       </c>
       <c r="BP17" s="5">
-        <f t="shared" si="14"/>
-        <v>91.048605588733551</v>
+        <f t="shared" si="18"/>
+        <v>90.692321780312454</v>
       </c>
       <c r="BQ17" s="5">
-        <f t="shared" si="14"/>
-        <v>90.138119532846218</v>
+        <f t="shared" si="18"/>
+        <v>89.785398562509329</v>
       </c>
       <c r="BR17" s="5">
-        <f t="shared" si="14"/>
-        <v>89.23673833751775</v>
+        <f t="shared" si="18"/>
+        <v>88.887544576884238</v>
       </c>
       <c r="BS17" s="5">
-        <f t="shared" si="14"/>
-        <v>88.344370954142576</v>
+        <f t="shared" si="18"/>
+        <v>87.998669131115392</v>
       </c>
       <c r="BT17" s="5">
-        <f t="shared" si="14"/>
-        <v>87.460927244601152</v>
+        <f t="shared" si="18"/>
+        <v>87.118682439804232</v>
       </c>
       <c r="BU17" s="5">
-        <f t="shared" si="14"/>
-        <v>86.586317972155143</v>
+        <f t="shared" si="18"/>
+        <v>86.247495615406194</v>
       </c>
       <c r="BV17" s="5">
-        <f t="shared" si="14"/>
-        <v>85.720454792433586</v>
+        <f t="shared" si="18"/>
+        <v>85.385020659252135</v>
       </c>
       <c r="BW17" s="5">
-        <f t="shared" si="14"/>
-        <v>84.863250244509246</v>
+        <f t="shared" si="18"/>
+        <v>84.531170452659609</v>
       </c>
       <c r="BX17" s="5">
-        <f t="shared" si="14"/>
-        <v>84.014617742064146</v>
+        <f t="shared" si="18"/>
+        <v>83.685858748133015</v>
       </c>
       <c r="BY17" s="5">
-        <f t="shared" si="14"/>
-        <v>83.174471564643511</v>
+        <f t="shared" si="18"/>
+        <v>82.849000160651684</v>
       </c>
       <c r="BZ17" s="5">
-        <f t="shared" si="14"/>
-        <v>82.342726848997074</v>
+        <f t="shared" si="18"/>
+        <v>82.020510159045173</v>
       </c>
       <c r="CA17" s="5">
-        <f t="shared" si="14"/>
-        <v>81.519299580507109</v>
+        <f t="shared" si="18"/>
+        <v>81.200305057454727</v>
       </c>
       <c r="CB17" s="5">
-        <f t="shared" si="14"/>
-        <v>80.704106584702032</v>
+        <f t="shared" si="18"/>
+        <v>80.388302006880181</v>
       </c>
       <c r="CC17" s="5">
-        <f t="shared" si="14"/>
-        <v>79.897065518855015</v>
+        <f t="shared" si="18"/>
+        <v>79.584418986811372</v>
       </c>
       <c r="CD17" s="5">
-        <f t="shared" si="14"/>
-        <v>79.098094863666461</v>
+        <f t="shared" si="18"/>
+        <v>78.788574796943251</v>
       </c>
       <c r="CE17" s="5">
-        <f t="shared" si="14"/>
-        <v>78.307113915029802</v>
+        <f t="shared" si="18"/>
+        <v>78.000689048973825</v>
       </c>
       <c r="CF17" s="5">
-        <f t="shared" si="14"/>
-        <v>77.524042775879508</v>
+        <f t="shared" si="18"/>
+        <v>77.220682158484081</v>
       </c>
       <c r="CG17" s="5">
-        <f t="shared" si="14"/>
-        <v>76.748802348120705</v>
+        <f t="shared" si="18"/>
+        <v>76.448475336899236</v>
       </c>
       <c r="CH17" s="5">
-        <f t="shared" si="14"/>
-        <v>75.981314324639499</v>
+        <f t="shared" si="18"/>
+        <v>75.683990583530246</v>
       </c>
       <c r="CI17" s="5">
-        <f t="shared" si="14"/>
-        <v>75.221501181393108</v>
+        <f t="shared" si="18"/>
+        <v>74.927150677694939</v>
       </c>
       <c r="CJ17" s="5">
-        <f t="shared" si="14"/>
-        <v>74.469286169579178</v>
+        <f t="shared" si="18"/>
+        <v>74.17787917091799</v>
       </c>
       <c r="CK17" s="5">
-        <f t="shared" si="14"/>
-        <v>73.724593307883381</v>
+        <f t="shared" si="18"/>
+        <v>73.43610037920881</v>
       </c>
       <c r="CL17" s="5">
-        <f t="shared" si="14"/>
-        <v>72.987347374804543</v>
+        <f t="shared" si="18"/>
+        <v>72.701739375416722</v>
       </c>
       <c r="CM17" s="5">
-        <f t="shared" si="14"/>
-        <v>72.2574739010565</v>
+        <f t="shared" si="18"/>
+        <v>71.974721981662555</v>
       </c>
       <c r="CN17" s="5">
-        <f t="shared" si="14"/>
-        <v>71.534899162045932</v>
+        <f t="shared" si="18"/>
+        <v>71.254974761845929</v>
       </c>
       <c r="CO17" s="5">
-        <f t="shared" si="14"/>
-        <v>70.819550170425472</v>
+        <f t="shared" si="18"/>
+        <v>70.542425014227476</v>
       </c>
       <c r="CP17" s="5">
-        <f t="shared" si="14"/>
-        <v>70.111354668721219</v>
+        <f t="shared" si="18"/>
+        <v>69.837000764085204</v>
       </c>
       <c r="CQ17" s="5">
-        <f t="shared" si="14"/>
-        <v>69.410241122034009</v>
+        <f t="shared" si="18"/>
+        <v>69.138630756444357</v>
       </c>
       <c r="CR17" s="5">
-        <f t="shared" si="14"/>
-        <v>68.716138710813667</v>
+        <f t="shared" si="18"/>
+        <v>68.447244448879914</v>
       </c>
       <c r="CS17" s="5">
-        <f t="shared" si="14"/>
-        <v>68.028977323705533</v>
+        <f t="shared" si="18"/>
+        <v>67.76277200439111</v>
       </c>
       <c r="CT17" s="5">
-        <f t="shared" si="14"/>
-        <v>67.348687550468483</v>
+        <f t="shared" si="18"/>
+        <v>67.085144284347194</v>
       </c>
       <c r="CU17" s="5">
-        <f t="shared" si="14"/>
-        <v>66.675200674963804</v>
+        <f t="shared" si="18"/>
+        <v>66.414292841503723</v>
       </c>
       <c r="CV17" s="5">
-        <f t="shared" si="14"/>
-        <v>66.008448668214172</v>
+        <f t="shared" si="18"/>
+        <v>65.750149913088691</v>
       </c>
       <c r="CW17" s="5">
-        <f t="shared" si="14"/>
-        <v>65.348364181532034</v>
+        <f t="shared" si="18"/>
+        <v>65.092648413957804</v>
       </c>
       <c r="CX17" s="5">
-        <f t="shared" si="14"/>
-        <v>64.694880539716706</v>
+        <f t="shared" si="18"/>
+        <v>64.441721929818229</v>
       </c>
       <c r="CY17" s="5">
-        <f t="shared" si="14"/>
-        <v>64.047931734319533</v>
+        <f t="shared" si="18"/>
+        <v>63.797304710520045</v>
       </c>
       <c r="CZ17" s="5">
-        <f t="shared" ref="CZ17:FK17" si="15">CY17*(1+$AQ$30)</f>
-        <v>63.407452416976341</v>
+        <f t="shared" ref="CZ17:FK17" si="19">CY17*(1+$AQ$30)</f>
+        <v>63.159331663414847</v>
       </c>
       <c r="DA17" s="5">
-        <f t="shared" si="15"/>
-        <v>62.773377892806579</v>
+        <f t="shared" si="19"/>
+        <v>62.527738346780694</v>
       </c>
       <c r="DB17" s="5">
-        <f t="shared" si="15"/>
-        <v>62.145644113878511</v>
+        <f t="shared" si="19"/>
+        <v>61.902460963312883</v>
       </c>
       <c r="DC17" s="5">
-        <f t="shared" si="15"/>
-        <v>61.524187672739728</v>
+        <f t="shared" si="19"/>
+        <v>61.283436353679754</v>
       </c>
       <c r="DD17" s="5">
-        <f t="shared" si="15"/>
-        <v>60.908945796012333</v>
+        <f t="shared" si="19"/>
+        <v>60.670601990142956</v>
       </c>
       <c r="DE17" s="5">
-        <f t="shared" si="15"/>
-        <v>60.299856338052209</v>
+        <f t="shared" si="19"/>
+        <v>60.063895970241525</v>
       </c>
       <c r="DF17" s="5">
-        <f t="shared" si="15"/>
-        <v>59.696857774671685</v>
+        <f t="shared" si="19"/>
+        <v>59.46325701053911</v>
       </c>
       <c r="DG17" s="5">
-        <f t="shared" si="15"/>
-        <v>59.09988919692497</v>
+        <f t="shared" si="19"/>
+        <v>58.86862444043372</v>
       </c>
       <c r="DH17" s="5">
-        <f t="shared" si="15"/>
-        <v>58.50889030495572</v>
+        <f t="shared" si="19"/>
+        <v>58.279938196029384</v>
       </c>
       <c r="DI17" s="5">
-        <f t="shared" si="15"/>
-        <v>57.923801401906161</v>
+        <f t="shared" si="19"/>
+        <v>57.697138814069092</v>
       </c>
       <c r="DJ17" s="5">
-        <f t="shared" si="15"/>
-        <v>57.344563387887099</v>
+        <f t="shared" si="19"/>
+        <v>57.1201674259284</v>
       </c>
       <c r="DK17" s="5">
-        <f t="shared" si="15"/>
-        <v>56.77111775400823</v>
+        <f t="shared" si="19"/>
+        <v>56.548965751669115</v>
       </c>
       <c r="DL17" s="5">
-        <f t="shared" si="15"/>
-        <v>56.203406576468147</v>
+        <f t="shared" si="19"/>
+        <v>55.983476094152422</v>
       </c>
       <c r="DM17" s="5">
-        <f t="shared" si="15"/>
-        <v>55.641372510703462</v>
+        <f t="shared" si="19"/>
+        <v>55.423641333210895</v>
       </c>
       <c r="DN17" s="5">
-        <f t="shared" si="15"/>
-        <v>55.084958785596427</v>
+        <f t="shared" si="19"/>
+        <v>54.869404919878782</v>
       </c>
       <c r="DO17" s="5">
-        <f t="shared" si="15"/>
-        <v>54.534109197740463</v>
+        <f t="shared" si="19"/>
+        <v>54.320710870679996</v>
       </c>
       <c r="DP17" s="5">
-        <f t="shared" si="15"/>
-        <v>53.988768105763057</v>
+        <f t="shared" si="19"/>
+        <v>53.777503761973193</v>
       </c>
       <c r="DQ17" s="5">
-        <f t="shared" si="15"/>
-        <v>53.448880424705429</v>
+        <f t="shared" si="19"/>
+        <v>53.239728724353462</v>
       </c>
       <c r="DR17" s="5">
-        <f t="shared" si="15"/>
-        <v>52.914391620458375</v>
+        <f t="shared" si="19"/>
+        <v>52.707331437109929</v>
       </c>
       <c r="DS17" s="5">
-        <f t="shared" si="15"/>
-        <v>52.385247704253793</v>
+        <f t="shared" si="19"/>
+        <v>52.180258122738827</v>
       </c>
       <c r="DT17" s="5">
-        <f t="shared" si="15"/>
-        <v>51.861395227211254</v>
+        <f t="shared" si="19"/>
+        <v>51.658455541511437</v>
       </c>
       <c r="DU17" s="5">
-        <f t="shared" si="15"/>
-        <v>51.342781274939142</v>
+        <f t="shared" si="19"/>
+        <v>51.141870986096322</v>
       </c>
       <c r="DV17" s="5">
-        <f t="shared" si="15"/>
-        <v>50.829353462189751</v>
+        <f t="shared" si="19"/>
+        <v>50.63045227623536</v>
       </c>
       <c r="DW17" s="5">
-        <f t="shared" si="15"/>
-        <v>50.321059927567852</v>
+        <f t="shared" si="19"/>
+        <v>50.124147753473004</v>
       </c>
       <c r="DX17" s="5">
-        <f t="shared" si="15"/>
-        <v>49.817849328292176</v>
+        <f t="shared" si="19"/>
+        <v>49.62290627593827</v>
       </c>
       <c r="DY17" s="5">
-        <f t="shared" si="15"/>
-        <v>49.319670835009255</v>
+        <f t="shared" si="19"/>
+        <v>49.126677213178887</v>
       </c>
       <c r="DZ17" s="5">
-        <f t="shared" si="15"/>
-        <v>48.826474126659164</v>
+        <f t="shared" si="19"/>
+        <v>48.6354104410471</v>
       </c>
       <c r="EA17" s="5">
-        <f t="shared" si="15"/>
-        <v>48.338209385392574</v>
+        <f t="shared" si="19"/>
+        <v>48.149056336636626</v>
       </c>
       <c r="EB17" s="5">
-        <f t="shared" si="15"/>
-        <v>47.854827291538648</v>
+        <f t="shared" si="19"/>
+        <v>47.667565773270262</v>
       </c>
       <c r="EC17" s="5">
-        <f t="shared" si="15"/>
-        <v>47.376279018623258</v>
+        <f t="shared" si="19"/>
+        <v>47.190890115537556</v>
       </c>
       <c r="ED17" s="5">
-        <f t="shared" si="15"/>
-        <v>46.902516228437023</v>
+        <f t="shared" si="19"/>
+        <v>46.718981214382183</v>
       </c>
       <c r="EE17" s="5">
-        <f t="shared" si="15"/>
-        <v>46.433491066152655</v>
+        <f t="shared" si="19"/>
+        <v>46.251791402238361</v>
       </c>
       <c r="EF17" s="5">
-        <f t="shared" si="15"/>
-        <v>45.969156155491127</v>
+        <f t="shared" si="19"/>
+        <v>45.789273488215976</v>
       </c>
       <c r="EG17" s="5">
-        <f t="shared" si="15"/>
-        <v>45.509464593936215</v>
+        <f t="shared" si="19"/>
+        <v>45.331380753333818</v>
       </c>
       <c r="EH17" s="5">
-        <f t="shared" si="15"/>
-        <v>45.054369947996854</v>
+        <f t="shared" si="19"/>
+        <v>44.878066945800477</v>
       </c>
       <c r="EI17" s="5">
-        <f t="shared" si="15"/>
-        <v>44.603826248516881</v>
+        <f t="shared" si="19"/>
+        <v>44.429286276342474</v>
       </c>
       <c r="EJ17" s="5">
-        <f t="shared" si="15"/>
-        <v>44.157787986031714</v>
+        <f t="shared" si="19"/>
+        <v>43.984993413579048</v>
       </c>
       <c r="EK17" s="5">
-        <f t="shared" si="15"/>
-        <v>43.716210106171395</v>
+        <f t="shared" si="19"/>
+        <v>43.545143479443254</v>
       </c>
       <c r="EL17" s="5">
-        <f t="shared" si="15"/>
-        <v>43.279048005109679</v>
+        <f t="shared" si="19"/>
+        <v>43.109692044648824</v>
       </c>
       <c r="EM17" s="5">
-        <f t="shared" si="15"/>
-        <v>42.846257525058583</v>
+        <f t="shared" si="19"/>
+        <v>42.678595124202339</v>
       </c>
       <c r="EN17" s="5">
-        <f t="shared" si="15"/>
-        <v>42.417794949807998</v>
+        <f t="shared" si="19"/>
+        <v>42.251809172960314</v>
       </c>
       <c r="EO17" s="5">
-        <f t="shared" si="15"/>
-        <v>41.993617000309918</v>
+        <f t="shared" si="19"/>
+        <v>41.829291081230714</v>
       </c>
       <c r="EP17" s="5">
-        <f t="shared" si="15"/>
-        <v>41.57368083030682</v>
+        <f t="shared" si="19"/>
+        <v>41.410998170418409</v>
       </c>
       <c r="EQ17" s="5">
-        <f t="shared" si="15"/>
-        <v>41.157944022003754</v>
+        <f t="shared" si="19"/>
+        <v>40.996888188714223</v>
       </c>
       <c r="ER17" s="5">
-        <f t="shared" si="15"/>
-        <v>40.746364581783716</v>
+        <f t="shared" si="19"/>
+        <v>40.586919306827077</v>
       </c>
       <c r="ES17" s="5">
-        <f t="shared" si="15"/>
-        <v>40.338900935965881</v>
+        <f t="shared" si="19"/>
+        <v>40.181050113758808</v>
       </c>
       <c r="ET17" s="5">
-        <f t="shared" si="15"/>
-        <v>39.935511926606225</v>
+        <f t="shared" si="19"/>
+        <v>39.779239612621218</v>
       </c>
       <c r="EU17" s="5">
-        <f t="shared" si="15"/>
-        <v>39.536156807340163</v>
+        <f t="shared" si="19"/>
+        <v>39.381447216495005</v>
       </c>
       <c r="EV17" s="5">
-        <f t="shared" si="15"/>
-        <v>39.140795239266758</v>
+        <f t="shared" si="19"/>
+        <v>38.987632744330057</v>
       </c>
       <c r="EW17" s="5">
-        <f t="shared" si="15"/>
-        <v>38.749387286874089</v>
+        <f t="shared" si="19"/>
+        <v>38.597756416886753</v>
       </c>
       <c r="EX17" s="5">
-        <f t="shared" si="15"/>
-        <v>38.361893414005351</v>
+        <f t="shared" si="19"/>
+        <v>38.211778852717885</v>
       </c>
       <c r="EY17" s="5">
-        <f t="shared" si="15"/>
-        <v>37.978274479865298</v>
+        <f t="shared" si="19"/>
+        <v>37.829661064190702</v>
       </c>
       <c r="EZ17" s="5">
-        <f t="shared" si="15"/>
-        <v>37.598491735066645</v>
+        <f t="shared" si="19"/>
+        <v>37.451364453548798</v>
       </c>
       <c r="FA17" s="5">
-        <f t="shared" si="15"/>
-        <v>37.222506817715981</v>
+        <f t="shared" si="19"/>
+        <v>37.076850809013308</v>
       </c>
       <c r="FB17" s="5">
-        <f t="shared" si="15"/>
-        <v>36.850281749538823</v>
+        <f t="shared" si="19"/>
+        <v>36.706082300923178</v>
       </c>
       <c r="FC17" s="5">
-        <f t="shared" si="15"/>
-        <v>36.481778932043433</v>
+        <f t="shared" si="19"/>
+        <v>36.339021477913946</v>
       </c>
       <c r="FD17" s="5">
-        <f t="shared" si="15"/>
-        <v>36.116961142723</v>
+        <f t="shared" si="19"/>
+        <v>35.975631263134808</v>
       </c>
       <c r="FE17" s="5">
-        <f t="shared" si="15"/>
-        <v>35.75579153129577</v>
+        <f t="shared" si="19"/>
+        <v>35.615874950503461</v>
       </c>
       <c r="FF17" s="5">
-        <f t="shared" si="15"/>
-        <v>35.398233615982811</v>
+        <f t="shared" si="19"/>
+        <v>35.259716200998426</v>
       </c>
       <c r="FG17" s="5">
-        <f t="shared" si="15"/>
-        <v>35.04425127982298</v>
+        <f t="shared" si="19"/>
+        <v>34.907119038988441</v>
       </c>
       <c r="FH17" s="5">
-        <f t="shared" si="15"/>
-        <v>34.693808767024748</v>
+        <f t="shared" si="19"/>
+        <v>34.558047848598555</v>
       </c>
       <c r="FI17" s="5">
-        <f t="shared" si="15"/>
-        <v>34.346870679354502</v>
+        <f t="shared" si="19"/>
+        <v>34.21246737011257</v>
       </c>
       <c r="FJ17" s="5">
-        <f t="shared" si="15"/>
-        <v>34.003401972560958</v>
+        <f t="shared" si="19"/>
+        <v>33.870342696411441</v>
       </c>
       <c r="FK17" s="5">
-        <f t="shared" si="15"/>
-        <v>33.663367952835351</v>
+        <f t="shared" si="19"/>
+        <v>33.531639269447325</v>
       </c>
       <c r="FL17" s="5">
-        <f t="shared" ref="FL17:HW17" si="16">FK17*(1+$AQ$30)</f>
-        <v>33.326734273306997</v>
+        <f t="shared" ref="FL17:HW17" si="20">FK17*(1+$AQ$30)</f>
+        <v>33.196322876752852</v>
       </c>
       <c r="FM17" s="5">
-        <f t="shared" si="16"/>
-        <v>32.993466930573923</v>
+        <f t="shared" si="20"/>
+        <v>32.864359647985324</v>
       </c>
       <c r="FN17" s="5">
-        <f t="shared" si="16"/>
-        <v>32.66353226126818</v>
+        <f t="shared" si="20"/>
+        <v>32.535716051505467</v>
       </c>
       <c r="FO17" s="5">
-        <f t="shared" si="16"/>
-        <v>32.336896938655499</v>
+        <f t="shared" si="20"/>
+        <v>32.210358890990413</v>
       </c>
       <c r="FP17" s="5">
-        <f t="shared" si="16"/>
-        <v>32.013527969268942</v>
+        <f t="shared" si="20"/>
+        <v>31.888255302080509</v>
       </c>
       <c r="FQ17" s="5">
-        <f t="shared" si="16"/>
-        <v>31.693392689576253</v>
+        <f t="shared" si="20"/>
+        <v>31.569372749059703</v>
       </c>
       <c r="FR17" s="5">
-        <f t="shared" si="16"/>
-        <v>31.376458762680489</v>
+        <f t="shared" si="20"/>
+        <v>31.253679021569106</v>
       </c>
       <c r="FS17" s="5">
-        <f t="shared" si="16"/>
-        <v>31.062694175053682</v>
+        <f t="shared" si="20"/>
+        <v>30.941142231353414</v>
       </c>
       <c r="FT17" s="5">
-        <f t="shared" si="16"/>
-        <v>30.752067233303144</v>
+        <f t="shared" si="20"/>
+        <v>30.63173080903988</v>
       </c>
       <c r="FU17" s="5">
-        <f t="shared" si="16"/>
-        <v>30.444546560970114</v>
+        <f t="shared" si="20"/>
+        <v>30.32541350094948</v>
       </c>
       <c r="FV17" s="5">
-        <f t="shared" si="16"/>
-        <v>30.140101095360411</v>
+        <f t="shared" si="20"/>
+        <v>30.022159365939984</v>
       </c>
       <c r="FW17" s="5">
-        <f t="shared" si="16"/>
-        <v>29.838700084406806</v>
+        <f t="shared" si="20"/>
+        <v>29.721937772280583</v>
       </c>
       <c r="FX17" s="5">
-        <f t="shared" si="16"/>
-        <v>29.540313083562737</v>
+        <f t="shared" si="20"/>
+        <v>29.424718394557775</v>
       </c>
       <c r="FY17" s="5">
-        <f t="shared" si="16"/>
-        <v>29.244909952727109</v>
+        <f t="shared" si="20"/>
+        <v>29.130471210612196</v>
       </c>
       <c r="FZ17" s="5">
-        <f t="shared" si="16"/>
-        <v>28.952460853199838</v>
+        <f t="shared" si="20"/>
+        <v>28.839166498506074</v>
       </c>
       <c r="GA17" s="5">
-        <f t="shared" si="16"/>
-        <v>28.66293624466784</v>
+        <f t="shared" si="20"/>
+        <v>28.550774833521015</v>
       </c>
       <c r="GB17" s="5">
-        <f t="shared" si="16"/>
-        <v>28.376306882221161</v>
+        <f t="shared" si="20"/>
+        <v>28.265267085185805</v>
       </c>
       <c r="GC17" s="5">
-        <f t="shared" si="16"/>
-        <v>28.092543813398951</v>
+        <f t="shared" si="20"/>
+        <v>27.982614414333945</v>
       </c>
       <c r="GD17" s="5">
-        <f t="shared" si="16"/>
-        <v>27.81161837526496</v>
+        <f t="shared" si="20"/>
+        <v>27.702788270190606</v>
       </c>
       <c r="GE17" s="5">
-        <f t="shared" si="16"/>
-        <v>27.533502191512309</v>
+        <f t="shared" si="20"/>
+        <v>27.425760387488701</v>
       </c>
       <c r="GF17" s="5">
-        <f t="shared" si="16"/>
-        <v>27.258167169597186</v>
+        <f t="shared" si="20"/>
+        <v>27.151502783613815</v>
       </c>
       <c r="GG17" s="5">
-        <f t="shared" si="16"/>
-        <v>26.985585497901216</v>
+        <f t="shared" si="20"/>
+        <v>26.879987755777677</v>
       </c>
       <c r="GH17" s="5">
-        <f t="shared" si="16"/>
-        <v>26.715729642922202</v>
+        <f t="shared" si="20"/>
+        <v>26.611187878219901</v>
       </c>
       <c r="GI17" s="5">
-        <f t="shared" si="16"/>
-        <v>26.448572346492981</v>
+        <f t="shared" si="20"/>
+        <v>26.345075999437704</v>
       </c>
       <c r="GJ17" s="5">
-        <f t="shared" si="16"/>
-        <v>26.184086623028051</v>
+        <f t="shared" si="20"/>
+        <v>26.081625239443326</v>
       </c>
       <c r="GK17" s="5">
-        <f t="shared" si="16"/>
-        <v>25.922245756797771</v>
+        <f t="shared" si="20"/>
+        <v>25.820808987048892</v>
       </c>
       <c r="GL17" s="5">
-        <f t="shared" si="16"/>
-        <v>25.663023299229792</v>
+        <f t="shared" si="20"/>
+        <v>25.562600897178402</v>
       </c>
       <c r="GM17" s="5">
-        <f t="shared" si="16"/>
-        <v>25.406393066237495</v>
+        <f t="shared" si="20"/>
+        <v>25.306974888206618</v>
       </c>
       <c r="GN17" s="5">
-        <f t="shared" si="16"/>
-        <v>25.152329135575119</v>
+        <f t="shared" si="20"/>
+        <v>25.053905139324552</v>
       </c>
       <c r="GO17" s="5">
-        <f t="shared" si="16"/>
-        <v>24.900805844219366</v>
+        <f t="shared" si="20"/>
+        <v>24.803366087931305</v>
       </c>
       <c r="GP17" s="5">
-        <f t="shared" si="16"/>
-        <v>24.651797785777173</v>
+        <f t="shared" si="20"/>
+        <v>24.555332427051994</v>
       </c>
       <c r="GQ17" s="5">
-        <f t="shared" si="16"/>
-        <v>24.405279807919403</v>
+        <f t="shared" si="20"/>
+        <v>24.309779102781473</v>
       </c>
       <c r="GR17" s="5">
-        <f t="shared" si="16"/>
-        <v>24.161227009840207</v>
+        <f t="shared" si="20"/>
+        <v>24.066681311753658</v>
       </c>
       <c r="GS17" s="5">
-        <f t="shared" si="16"/>
-        <v>23.919614739741803</v>
+        <f t="shared" si="20"/>
+        <v>23.826014498636123</v>
       </c>
       <c r="GT17" s="5">
-        <f t="shared" si="16"/>
-        <v>23.680418592344385</v>
+        <f t="shared" si="20"/>
+        <v>23.58775435364976</v>
       </c>
       <c r="GU17" s="5">
-        <f t="shared" si="16"/>
-        <v>23.443614406420942</v>
+        <f t="shared" si="20"/>
+        <v>23.351876810113264</v>
       </c>
       <c r="GV17" s="5">
-        <f t="shared" si="16"/>
-        <v>23.209178262356733</v>
+        <f t="shared" si="20"/>
+        <v>23.118358042012133</v>
       </c>
       <c r="GW17" s="5">
-        <f t="shared" si="16"/>
-        <v>22.977086479733167</v>
+        <f t="shared" si="20"/>
+        <v>22.887174461592011</v>
       </c>
       <c r="GX17" s="5">
-        <f t="shared" si="16"/>
-        <v>22.747315614935836</v>
+        <f t="shared" si="20"/>
+        <v>22.658302716976092</v>
       </c>
       <c r="GY17" s="5">
-        <f t="shared" si="16"/>
-        <v>22.519842458786478</v>
+        <f t="shared" si="20"/>
+        <v>22.431719689806332</v>
       </c>
       <c r="GZ17" s="5">
-        <f t="shared" si="16"/>
-        <v>22.294644034198612</v>
+        <f t="shared" si="20"/>
+        <v>22.207402492908269</v>
       </c>
       <c r="HA17" s="5">
-        <f t="shared" si="16"/>
-        <v>22.071697593856626</v>
+        <f t="shared" si="20"/>
+        <v>21.985328467979187</v>
       </c>
       <c r="HB17" s="5">
-        <f t="shared" si="16"/>
-        <v>21.850980617918061</v>
+        <f t="shared" si="20"/>
+        <v>21.765475183299394</v>
       </c>
       <c r="HC17" s="5">
-        <f t="shared" si="16"/>
-        <v>21.63247081173888</v>
+        <f t="shared" si="20"/>
+        <v>21.547820431466398</v>
       </c>
       <c r="HD17" s="5">
-        <f t="shared" si="16"/>
-        <v>21.41614610362149</v>
+        <f t="shared" si="20"/>
+        <v>21.332342227151734</v>
       </c>
       <c r="HE17" s="5">
-        <f t="shared" si="16"/>
-        <v>21.201984642585273</v>
+        <f t="shared" si="20"/>
+        <v>21.119018804880216</v>
       </c>
       <c r="HF17" s="5">
-        <f t="shared" si="16"/>
-        <v>20.98996479615942</v>
+        <f t="shared" si="20"/>
+        <v>20.907828616831413</v>
       </c>
       <c r="HG17" s="5">
-        <f t="shared" si="16"/>
-        <v>20.780065148197824</v>
+        <f t="shared" si="20"/>
+        <v>20.698750330663099</v>
       </c>
       <c r="HH17" s="5">
-        <f t="shared" si="16"/>
-        <v>20.572264496715846</v>
+        <f t="shared" si="20"/>
+        <v>20.491762827356467</v>
       </c>
       <c r="HI17" s="5">
-        <f t="shared" si="16"/>
-        <v>20.366541851748686</v>
+        <f t="shared" si="20"/>
+        <v>20.286845199082901</v>
       </c>
       <c r="HJ17" s="5">
-        <f t="shared" si="16"/>
-        <v>20.162876433231197</v>
+        <f t="shared" si="20"/>
+        <v>20.083976747092073</v>
       </c>
       <c r="HK17" s="5">
-        <f t="shared" si="16"/>
-        <v>19.961247668898885</v>
+        <f t="shared" si="20"/>
+        <v>19.883136979621153</v>
       </c>
       <c r="HL17" s="5">
-        <f t="shared" si="16"/>
-        <v>19.761635192209894</v>
+        <f t="shared" si="20"/>
+        <v>19.684305609824939</v>
       </c>
       <c r="HM17" s="5">
-        <f t="shared" si="16"/>
-        <v>19.564018840287794</v>
+        <f t="shared" si="20"/>
+        <v>19.48746255372669</v>
       </c>
       <c r="HN17" s="5">
-        <f t="shared" si="16"/>
-        <v>19.368378651884917</v>
+        <f t="shared" si="20"/>
+        <v>19.292587928189423</v>
       </c>
       <c r="HO17" s="5">
-        <f t="shared" si="16"/>
-        <v>19.174694865366067</v>
+        <f t="shared" si="20"/>
+        <v>19.099662048907529</v>
       </c>
       <c r="HP17" s="5">
-        <f t="shared" si="16"/>
-        <v>18.982947916712405</v>
+        <f t="shared" si="20"/>
+        <v>18.908665428418452</v>
       </c>
       <c r="HQ17" s="5">
-        <f t="shared" si="16"/>
-        <v>18.793118437545282</v>
+        <f t="shared" si="20"/>
+        <v>18.719578774134266</v>
       </c>
       <c r="HR17" s="5">
-        <f t="shared" si="16"/>
-        <v>18.605187253169827</v>
+        <f t="shared" si="20"/>
+        <v>18.532382986392925</v>
       </c>
       <c r="HS17" s="5">
-        <f t="shared" si="16"/>
-        <v>18.419135380638128</v>
+        <f t="shared" si="20"/>
+        <v>18.347059156528996</v>
       </c>
       <c r="HT17" s="5">
-        <f t="shared" si="16"/>
-        <v>18.234944026831748</v>
+        <f t="shared" si="20"/>
+        <v>18.163588564963707</v>
       </c>
       <c r="HU17" s="5">
-        <f t="shared" si="16"/>
-        <v>18.05259458656343</v>
+        <f t="shared" si="20"/>
+        <v>17.98195267931407</v>
       </c>
       <c r="HV17" s="5">
-        <f t="shared" si="16"/>
-        <v>17.872068640697794</v>
+        <f t="shared" si="20"/>
+        <v>17.802133152520927</v>
       </c>
       <c r="HW17" s="5">
-        <f t="shared" si="16"/>
-        <v>17.693347954290815</v>
+        <f t="shared" si="20"/>
+        <v>17.624111820995719</v>
       </c>
       <c r="HX17" s="5">
-        <f t="shared" ref="HX17:KI17" si="17">HW17*(1+$AQ$30)</f>
-        <v>17.516414474747908</v>
+        <f t="shared" ref="HX17:KI17" si="21">HW17*(1+$AQ$30)</f>
+        <v>17.44787070278576</v>
       </c>
       <c r="HY17" s="5">
-        <f t="shared" si="17"/>
-        <v>17.341250330000427</v>
+        <f t="shared" si="21"/>
+        <v>17.273391995757901</v>
       </c>
       <c r="HZ17" s="5">
-        <f t="shared" si="17"/>
-        <v>17.167837826700424</v>
+        <f t="shared" si="21"/>
+        <v>17.100658075800322</v>
       </c>
       <c r="IA17" s="5">
-        <f t="shared" si="17"/>
-        <v>16.996159448433421</v>
+        <f t="shared" si="21"/>
+        <v>16.929651495042318</v>
       </c>
       <c r="IB17" s="5">
-        <f t="shared" si="17"/>
-        <v>16.826197853949086</v>
+        <f t="shared" si="21"/>
+        <v>16.760354980091893</v>
       </c>
       <c r="IC17" s="5">
-        <f t="shared" si="17"/>
-        <v>16.657935875409596</v>
+        <f t="shared" si="21"/>
+        <v>16.592751430290974</v>
       </c>
       <c r="ID17" s="5">
-        <f t="shared" si="17"/>
-        <v>16.4913565166555</v>
+        <f t="shared" si="21"/>
+        <v>16.426823915988063</v>
       </c>
       <c r="IE17" s="5">
-        <f t="shared" si="17"/>
-        <v>16.326442951488946</v>
+        <f t="shared" si="21"/>
+        <v>16.262555676828182</v>
       </c>
       <c r="IF17" s="5">
-        <f t="shared" si="17"/>
-        <v>16.163178521974057</v>
+        <f t="shared" si="21"/>
+        <v>16.099930120059899</v>
       </c>
       <c r="IG17" s="5">
-        <f t="shared" si="17"/>
-        <v>16.001546736754317</v>
+        <f t="shared" si="21"/>
+        <v>15.9389308188593</v>
       </c>
       <c r="IH17" s="5">
-        <f t="shared" si="17"/>
-        <v>15.841531269386774</v>
+        <f t="shared" si="21"/>
+        <v>15.779541510670706</v>
       </c>
       <c r="II17" s="5">
-        <f t="shared" si="17"/>
-        <v>15.683115956692907</v>
+        <f t="shared" si="21"/>
+        <v>15.621746095563999</v>
       </c>
       <c r="IJ17" s="5">
-        <f t="shared" si="17"/>
-        <v>15.526284797125978</v>
+        <f t="shared" si="21"/>
+        <v>15.46552863460836</v>
       </c>
       <c r="IK17" s="5">
-        <f t="shared" si="17"/>
-        <v>15.371021949154718</v>
+        <f t="shared" si="21"/>
+        <v>15.310873348262275</v>
       </c>
       <c r="IL17" s="5">
-        <f t="shared" si="17"/>
-        <v>15.217311729663171</v>
+        <f t="shared" si="21"/>
+        <v>15.157764614779651</v>
       </c>
       <c r="IM17" s="5">
-        <f t="shared" si="17"/>
-        <v>15.065138612366539</v>
+        <f t="shared" si="21"/>
+        <v>15.006186968631855</v>
       </c>
       <c r="IN17" s="5">
-        <f t="shared" si="17"/>
-        <v>14.914487226242873</v>
+        <f t="shared" si="21"/>
+        <v>14.856125098945537</v>
       </c>
       <c r="IO17" s="5">
-        <f t="shared" si="17"/>
-        <v>14.765342353980444</v>
+        <f t="shared" si="21"/>
+        <v>14.707563847956081</v>
       </c>
       <c r="IP17" s="5">
-        <f t="shared" si="17"/>
-        <v>14.617688930440639</v>
+        <f t="shared" si="21"/>
+        <v>14.560488209476519</v>
       </c>
       <c r="IQ17" s="5">
-        <f t="shared" si="17"/>
-        <v>14.471512041136233</v>
+        <f t="shared" si="21"/>
+        <v>14.414883327381753</v>
       </c>
       <c r="IR17" s="5">
-        <f t="shared" si="17"/>
-        <v>14.32679692072487</v>
+        <f t="shared" si="21"/>
+        <v>14.270734494107936</v>
       </c>
       <c r="IS17" s="5">
-        <f t="shared" si="17"/>
-        <v>14.183528951517621</v>
+        <f t="shared" si="21"/>
+        <v>14.128027149166856</v>
       </c>
       <c r="IT17" s="5">
-        <f t="shared" si="17"/>
-        <v>14.041693662002444</v>
+        <f t="shared" si="21"/>
+        <v>13.986746877675188</v>
       </c>
       <c r="IU17" s="5">
-        <f t="shared" si="17"/>
-        <v>13.90127672538242</v>
+        <f t="shared" si="21"/>
+        <v>13.846879408898436</v>
       </c>
       <c r="IV17" s="5">
-        <f t="shared" si="17"/>
-        <v>13.762263958128596</v>
+        <f t="shared" si="21"/>
+        <v>13.708410614809452</v>
       </c>
       <c r="IW17" s="5">
-        <f t="shared" si="17"/>
-        <v>13.62464131854731</v>
+        <f t="shared" si="21"/>
+        <v>13.571326508661357</v>
       </c>
       <c r="IX17" s="5">
-        <f t="shared" si="17"/>
-        <v>13.488394905361837</v>
+        <f t="shared" si="21"/>
+        <v>13.435613243574744</v>
       </c>
       <c r="IY17" s="5">
-        <f t="shared" si="17"/>
-        <v>13.353510956308218</v>
+        <f t="shared" si="21"/>
+        <v>13.301257111138996</v>
       </c>
       <c r="IZ17" s="5">
-        <f t="shared" si="17"/>
-        <v>13.219975846745136</v>
+        <f t="shared" si="21"/>
+        <v>13.168244540027606</v>
       </c>
       <c r="JA17" s="5">
-        <f t="shared" si="17"/>
-        <v>13.087776088277684</v>
+        <f t="shared" si="21"/>
+        <v>13.03656209462733</v>
       </c>
       <c r="JB17" s="5">
-        <f t="shared" si="17"/>
-        <v>12.956898327394907</v>
+        <f t="shared" si="21"/>
+        <v>12.906196473681057</v>
       </c>
       <c r="JC17" s="5">
-        <f t="shared" si="17"/>
-        <v>12.827329344120958</v>
+        <f t="shared" si="21"/>
+        <v>12.777134508944245</v>
       </c>
       <c r="JD17" s="5">
-        <f t="shared" si="17"/>
-        <v>12.699056050679749</v>
+        <f t="shared" si="21"/>
+        <v>12.649363163854803</v>
       </c>
       <c r="JE17" s="5">
-        <f t="shared" si="17"/>
-        <v>12.572065490172951</v>
+        <f t="shared" si="21"/>
+        <v>12.522869532216255</v>
       </c>
       <c r="JF17" s="5">
-        <f t="shared" si="17"/>
-        <v>12.446344835271221</v>
+        <f t="shared" si="21"/>
+        <v>12.397640836894093</v>
       </c>
       <c r="JG17" s="5">
-        <f t="shared" si="17"/>
-        <v>12.321881386918509</v>
+        <f t="shared" si="21"/>
+        <v>12.273664428525151</v>
       </c>
       <c r="JH17" s="5">
-        <f t="shared" si="17"/>
-        <v>12.198662573049324</v>
+        <f t="shared" si="21"/>
+        <v>12.150927784239899</v>
       </c>
       <c r="JI17" s="5">
-        <f t="shared" si="17"/>
-        <v>12.076675947318831</v>
+        <f t="shared" si="21"/>
+        <v>12.0294185063975</v>
       </c>
       <c r="JJ17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.955909187845643</v>
+        <f t="shared" si="21"/>
+        <v>11.909124321333525</v>
       </c>
       <c r="JK17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.836350095967187</v>
+        <f t="shared" si="21"/>
+        <v>11.790033078120191</v>
       </c>
       <c r="JL17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.717986595007515</v>
+        <f t="shared" si="21"/>
+        <v>11.672132747338988</v>
       </c>
       <c r="JM17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.600806729057441</v>
+        <f t="shared" si="21"/>
+        <v>11.555411419865598</v>
       </c>
       <c r="JN17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.484798661766867</v>
+        <f t="shared" si="21"/>
+        <v>11.439857305666942</v>
       </c>
       <c r="JO17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.369950675149198</v>
+        <f t="shared" si="21"/>
+        <v>11.325458732610272</v>
       </c>
       <c r="JP17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.256251168397705</v>
+        <f t="shared" si="21"/>
+        <v>11.21220414528417</v>
       </c>
       <c r="JQ17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.143688656713728</v>
+        <f t="shared" si="21"/>
+        <v>11.100082103831328</v>
       </c>
       <c r="JR17" s="5">
-        <f t="shared" si="17"/>
-        <v>11.032251770146591</v>
+        <f t="shared" si="21"/>
+        <v>10.989081282793014</v>
       </c>
       <c r="JS17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.921929252445125</v>
+        <f t="shared" si="21"/>
+        <v>10.879190469965085</v>
       </c>
       <c r="JT17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.812709959920673</v>
+        <f t="shared" si="21"/>
+        <v>10.770398565265435</v>
       </c>
       <c r="JU17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.704582860321466</v>
+        <f t="shared" si="21"/>
+        <v>10.662694579612781</v>
       </c>
       <c r="JV17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.597537031718252</v>
+        <f t="shared" si="21"/>
+        <v>10.556067633816653</v>
       </c>
       <c r="JW17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.49156166140107</v>
+        <f t="shared" si="21"/>
+        <v>10.450506957478487</v>
       </c>
       <c r="JX17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.386646044787058</v>
+        <f t="shared" si="21"/>
+        <v>10.346001887903702</v>
       </c>
       <c r="JY17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.282779584339188</v>
+        <f t="shared" si="21"/>
+        <v>10.242541869024665</v>
       </c>
       <c r="JZ17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.179951788495796</v>
+        <f t="shared" si="21"/>
+        <v>10.140116450334418</v>
       </c>
       <c r="KA17" s="5">
-        <f t="shared" si="17"/>
-        <v>10.078152270610838</v>
+        <f t="shared" si="21"/>
+        <v>10.038715285831074</v>
       </c>
       <c r="KB17" s="5">
-        <f t="shared" si="17"/>
-        <v>9.9773707479047289</v>
+        <f t="shared" si="21"/>
+        <v>9.9383281329727637</v>
       </c>
       <c r="KC17" s="5">
-        <f t="shared" si="17"/>
-        <v>9.8775970404256821</v>
+        <f t="shared" si="21"/>
+        <v>9.8389448516430367</v>
       </c>
       <c r="KD17" s="5">
-        <f t="shared" si="17"/>
-        <v>9.7788210700214258</v>
+        <f t="shared" si="21"/>
+        <v>9.7405554031266064</v>
       </c>
       <c r="KE17" s="5">
-        <f t="shared" si="17"/>
-        <v>9.6810328593212116</v>
+        <f t="shared" si="21"/>
+        <v>9.6431498490953409</v>
       </c>
       <c r="KF17" s="5">
-        <f t="shared" si="17"/>
-        <v>9.5842225307279989</v>
+        <f t="shared" si="21"/>
+        <v>9.5467183506043867</v>
       </c>
       <c r="KG17" s="5">
-        <f t="shared" si="17"/>
-        <v>9.4883803054207192</v>
+        <f t="shared" si="21"/>
+        <v>9.4512511670983432</v>
       </c>
       <c r="KH17" s="5">
-        <f t="shared" si="17"/>
-        <v>9.3934965023665118</v>
+        <f t="shared" si="21"/>
+        <v>9.3567386554273604</v>
       </c>
       <c r="KI17" s="5">
-        <f t="shared" si="17"/>
-        <v>9.2995615373428464</v>
+        <f t="shared" si="21"/>
+        <v>9.2631712688730872</v>
       </c>
       <c r="KJ17" s="5">
-        <f t="shared" ref="KJ17:MU17" si="18">KI17*(1+$AQ$30)</f>
-        <v>9.2065659219694176</v>
+        <f t="shared" ref="KJ17:MU17" si="22">KI17*(1+$AQ$30)</f>
+        <v>9.170539556184357</v>
       </c>
       <c r="KK17" s="5">
-        <f t="shared" si="18"/>
-        <v>9.1145002627497238</v>
+        <f t="shared" si="22"/>
+        <v>9.0788341606225131</v>
       </c>
       <c r="KL17" s="5">
-        <f t="shared" si="18"/>
-        <v>9.0233552601222264</v>
+        <f t="shared" si="22"/>
+        <v>8.9880458190162873</v>
       </c>
       <c r="KM17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.9331217075210034</v>
+        <f t="shared" si="22"/>
+        <v>8.8981653608261251</v>
       </c>
       <c r="KN17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.8437904904457927</v>
+        <f t="shared" si="22"/>
+        <v>8.8091837072178638</v>
       </c>
       <c r="KO17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.7553525855413348</v>
+        <f t="shared" si="22"/>
+        <v>8.7210918701456848</v>
       </c>
       <c r="KP17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.6677990596859207</v>
+        <f t="shared" si="22"/>
+        <v>8.6338809514442278</v>
       </c>
       <c r="KQ17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.5811210690890611</v>
+        <f t="shared" si="22"/>
+        <v>8.5475421419297852</v>
       </c>
       <c r="KR17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.495309858398171</v>
+        <f t="shared" si="22"/>
+        <v>8.4620667205104869</v>
       </c>
       <c r="KS17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.4103567598141886</v>
+        <f t="shared" si="22"/>
+        <v>8.3774460533053823</v>
       </c>
       <c r="KT17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.326253192216047</v>
+        <f t="shared" si="22"/>
+        <v>8.2936715927723288</v>
       </c>
       <c r="KU17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.2429906602938861</v>
+        <f t="shared" si="22"/>
+        <v>8.2107348768446062</v>
       </c>
       <c r="KV17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.1605607536909464</v>
+        <f t="shared" si="22"/>
+        <v>8.1286275280761604</v>
       </c>
       <c r="KW17" s="5">
-        <f t="shared" si="18"/>
-        <v>8.078955146154037</v>
+        <f t="shared" si="22"/>
+        <v>8.0473412527953982</v>
       </c>
       <c r="KX17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.9981655946924963</v>
+        <f t="shared" si="22"/>
+        <v>7.9668678402674438</v>
       </c>
       <c r="KY17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.918183938745571</v>
+        <f t="shared" si="22"/>
+        <v>7.8871991618647694</v>
       </c>
       <c r="KZ17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.8390020993581153</v>
+        <f t="shared" si="22"/>
+        <v>7.8083271702461214</v>
       </c>
       <c r="LA17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.7606120783645345</v>
+        <f t="shared" si="22"/>
+        <v>7.7302438985436606</v>
       </c>
       <c r="LB17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.6830059575808889</v>
+        <f t="shared" si="22"/>
+        <v>7.6529414595582237</v>
       </c>
       <c r="LC17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.6061758980050795</v>
+        <f t="shared" si="22"/>
+        <v>7.5764120449626411</v>
       </c>
       <c r="LD17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.530114139025029</v>
+        <f t="shared" si="22"/>
+        <v>7.5006479245130144</v>
       </c>
       <c r="LE17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.4548129976347788</v>
+        <f t="shared" si="22"/>
+        <v>7.4256414452678845</v>
       </c>
       <c r="LF17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.3802648676584308</v>
+        <f t="shared" si="22"/>
+        <v>7.351385030815206</v>
       </c>
       <c r="LG17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.3064622189818467</v>
+        <f t="shared" si="22"/>
+        <v>7.2778711805070539</v>
       </c>
       <c r="LH17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.2333975967920283</v>
+        <f t="shared" si="22"/>
+        <v>7.2050924687019835</v>
       </c>
       <c r="LI17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.1610636208241081</v>
+        <f t="shared" si="22"/>
+        <v>7.1330415440149633</v>
       </c>
       <c r="LJ17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.0894529846158667</v>
+        <f t="shared" si="22"/>
+        <v>7.0617111285748138</v>
       </c>
       <c r="LK17" s="5">
-        <f t="shared" si="18"/>
-        <v>7.0185584547697077</v>
+        <f t="shared" si="22"/>
+        <v>6.9910940172890657</v>
       </c>
       <c r="LL17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.9483728702220109</v>
+        <f t="shared" si="22"/>
+        <v>6.9211830771161749</v>
       </c>
       <c r="LM17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.8788891415197906</v>
+        <f t="shared" si="22"/>
+        <v>6.8519712463450126</v>
       </c>
       <c r="LN17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.8101002501045924</v>
+        <f t="shared" si="22"/>
+        <v>6.7834515338815624</v>
       </c>
       <c r="LO17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.7419992476035464</v>
+        <f t="shared" si="22"/>
+        <v>6.7156170185427468</v>
       </c>
       <c r="LP17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.6745792551275107</v>
+        <f t="shared" si="22"/>
+        <v>6.6484608483573195</v>
       </c>
       <c r="LQ17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.6078334625762354</v>
+        <f t="shared" si="22"/>
+        <v>6.5819762398737467</v>
       </c>
       <c r="LR17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.5417551279504726</v>
+        <f t="shared" si="22"/>
+        <v>6.5161564774750094</v>
       </c>
       <c r="LS17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.4763375766709679</v>
+        <f t="shared" si="22"/>
+        <v>6.450994912700259</v>
       </c>
       <c r="LT17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.4115742009042584</v>
+        <f t="shared" si="22"/>
+        <v>6.3864849635732561</v>
       </c>
       <c r="LU17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.3474584588952156</v>
+        <f t="shared" si="22"/>
+        <v>6.3226201139375231</v>
       </c>
       <c r="LV17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.283983874306263</v>
+        <f t="shared" si="22"/>
+        <v>6.2593939127981475</v>
       </c>
       <c r="LW17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.2211440355632002</v>
+        <f t="shared" si="22"/>
+        <v>6.1967999736701662</v>
       </c>
       <c r="LX17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.1589325952075678</v>
+        <f t="shared" si="22"/>
+        <v>6.1348319739334647</v>
       </c>
       <c r="LY17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.0973432692554921</v>
+        <f t="shared" si="22"/>
+        <v>6.0734836541941304</v>
       </c>
       <c r="LZ17" s="5">
-        <f t="shared" si="18"/>
-        <v>6.0363698365629368</v>
+        <f t="shared" si="22"/>
+        <v>6.0127488176521888</v>
       </c>
       <c r="MA17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.9760061381973077</v>
+        <f t="shared" si="22"/>
+        <v>5.9526213294756669</v>
       </c>
       <c r="MB17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.9162460768153347</v>
+        <f t="shared" si="22"/>
+        <v>5.89309511618091</v>
       </c>
       <c r="MC17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.8570836160471815</v>
+        <f t="shared" si="22"/>
+        <v>5.834164165019101</v>
       </c>
       <c r="MD17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.7985127798867095</v>
+        <f t="shared" si="22"/>
+        <v>5.7758225233689098</v>
       </c>
       <c r="ME17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.7405276520878425</v>
+        <f t="shared" si="22"/>
+        <v>5.7180642981352205</v>
       </c>
       <c r="MF17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.6831223755669642</v>
+        <f t="shared" si="22"/>
+        <v>5.6608836551538682</v>
       </c>
       <c r="MG17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.6262911518112944</v>
+        <f t="shared" si="22"/>
+        <v>5.6042748186023292</v>
       </c>
       <c r="MH17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.5700282402931816</v>
+        <f t="shared" si="22"/>
+        <v>5.5482320704163062</v>
       </c>
       <c r="MI17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.5143279578902495</v>
+        <f t="shared" si="22"/>
+        <v>5.4927497497121429</v>
       </c>
       <c r="MJ17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.4591846783113471</v>
+        <f t="shared" si="22"/>
+        <v>5.437822252215021</v>
       </c>
       <c r="MK17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.4045928315282339</v>
+        <f t="shared" si="22"/>
+        <v>5.3834440296928712</v>
       </c>
       <c r="ML17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.3505469032129511</v>
+        <f t="shared" si="22"/>
+        <v>5.3296095893959423</v>
       </c>
       <c r="MM17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.2970414341808212</v>
+        <f t="shared" si="22"/>
+        <v>5.2763134935019824</v>
       </c>
       <c r="MN17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.244071019839013</v>
+        <f t="shared" si="22"/>
+        <v>5.2235503585669623</v>
       </c>
       <c r="MO17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.1916303096406224</v>
+        <f t="shared" si="22"/>
+        <v>5.1713148549812926</v>
       </c>
       <c r="MP17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.1397140065442164</v>
+        <f t="shared" si="22"/>
+        <v>5.1196017064314798</v>
       </c>
       <c r="MQ17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.0883168664787739</v>
+        <f t="shared" si="22"/>
+        <v>5.0684056893671654</v>
       </c>
       <c r="MR17" s="5">
-        <f t="shared" si="18"/>
-        <v>5.0374336978139862</v>
+        <f t="shared" si="22"/>
+        <v>5.0177216324734939</v>
       </c>
       <c r="MS17" s="5">
-        <f t="shared" si="18"/>
-        <v>4.987059360835846</v>
+        <f t="shared" si="22"/>
+        <v>4.9675444161487592</v>
       </c>
       <c r="MT17" s="5">
-        <f t="shared" si="18"/>
-        <v>4.9371887672274877</v>
+        <f t="shared" si="22"/>
+        <v>4.9178689719872715</v>
       </c>
       <c r="MU17" s="5">
-        <f t="shared" si="18"/>
-        <v>4.8878168795552126</v>
+        <f t="shared" si="22"/>
+        <v>4.8686902822673988</v>
       </c>
       <c r="MV17" s="5">
-        <f t="shared" ref="MV17:OX17" si="19">MU17*(1+$AQ$30)</f>
-        <v>4.8389387107596606</v>
+        <f t="shared" ref="MV17:OX17" si="23">MU17*(1+$AQ$30)</f>
+        <v>4.8200033794447243</v>
       </c>
       <c r="MW17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.7905493236520638</v>
+        <f t="shared" si="23"/>
+        <v>4.7718033456502766</v>
       </c>
       <c r="MX17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.7426438304155427</v>
+        <f t="shared" si="23"/>
+        <v>4.7240853121937736</v>
       </c>
       <c r="MY17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.6952173921113873</v>
+        <f t="shared" si="23"/>
+        <v>4.6768444590718357</v>
       </c>
       <c r="MZ17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.6482652181902733</v>
+        <f t="shared" si="23"/>
+        <v>4.6300760144811175</v>
       </c>
       <c r="NA17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.6017825660083709</v>
+        <f t="shared" si="23"/>
+        <v>4.5837752543363059</v>
       </c>
       <c r="NB17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.5557647403482875</v>
+        <f t="shared" si="23"/>
+        <v>4.5379375017929426</v>
       </c>
       <c r="NC17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.5102070929448042</v>
+        <f t="shared" si="23"/>
+        <v>4.4925581267750134</v>
       </c>
       <c r="ND17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.4651050220153561</v>
+        <f t="shared" si="23"/>
+        <v>4.4476325455072629</v>
       </c>
       <c r="NE17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.4204539717952027</v>
+        <f t="shared" si="23"/>
+        <v>4.4031562200521899</v>
       </c>
       <c r="NF17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.3762494320772509</v>
+        <f t="shared" si="23"/>
+        <v>4.3591246578516678</v>
       </c>
       <c r="NG17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.3324869377564781</v>
+        <f t="shared" si="23"/>
+        <v>4.3155334112731509</v>
       </c>
       <c r="NH17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.2891620683789133</v>
+        <f t="shared" si="23"/>
+        <v>4.2723780771604192</v>
       </c>
       <c r="NI17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.2462704476951245</v>
+        <f t="shared" si="23"/>
+        <v>4.2296542963888148</v>
       </c>
       <c r="NJ17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.2038077432181735</v>
+        <f t="shared" si="23"/>
+        <v>4.1873577534249264</v>
       </c>
       <c r="NK17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.1617696657859922</v>
+        <f t="shared" si="23"/>
+        <v>4.1454841758906769</v>
       </c>
       <c r="NL17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.1201519691281323</v>
+        <f t="shared" si="23"/>
+        <v>4.10402933413177</v>
       </c>
       <c r="NM17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.0789504494368511</v>
+        <f t="shared" si="23"/>
+        <v>4.0629890407904519</v>
       </c>
       <c r="NN17" s="5">
-        <f t="shared" si="19"/>
-        <v>4.0381609449424829</v>
+        <f t="shared" si="23"/>
+        <v>4.0223591503825471</v>
       </c>
       <c r="NO17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.9977793354930582</v>
+        <f t="shared" si="23"/>
+        <v>3.9821355588787215</v>
       </c>
       <c r="NP17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.9578015421381276</v>
+        <f t="shared" si="23"/>
+        <v>3.9423142032899343</v>
       </c>
       <c r="NQ17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.9182235267167465</v>
+        <f t="shared" si="23"/>
+        <v>3.9028910612570349</v>
       </c>
       <c r="NR17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.8790412914495791</v>
+        <f t="shared" si="23"/>
+        <v>3.8638621506444646</v>
       </c>
       <c r="NS17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.8402508785350831</v>
+        <f t="shared" si="23"/>
+        <v>3.8252235291380199</v>
       </c>
       <c r="NT17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.8018483697497323</v>
+        <f t="shared" si="23"/>
+        <v>3.7869712938466398</v>
       </c>
       <c r="NU17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.763829886052235</v>
+        <f t="shared" si="23"/>
+        <v>3.7491015809081731</v>
       </c>
       <c r="NV17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.7261915871917126</v>
+        <f t="shared" si="23"/>
+        <v>3.7116105650990914</v>
       </c>
       <c r="NW17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.6889296713197957</v>
+        <f t="shared" si="23"/>
+        <v>3.6744944594481006</v>
       </c>
       <c r="NX17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.6520403746065977</v>
+        <f t="shared" si="23"/>
+        <v>3.6377495148536196</v>
       </c>
       <c r="NY17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.6155199708605319</v>
+        <f t="shared" si="23"/>
+        <v>3.6013720197050834</v>
       </c>
       <c r="NZ17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.5793647711519267</v>
+        <f t="shared" si="23"/>
+        <v>3.5653582995080324</v>
       </c>
       <c r="OA17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.5435711234404073</v>
+        <f t="shared" si="23"/>
+        <v>3.5297047165129523</v>
       </c>
       <c r="OB17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.5081354122060033</v>
+        <f t="shared" si="23"/>
+        <v>3.4944076693478228</v>
       </c>
       <c r="OC17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.4730540580839433</v>
+        <f t="shared" si="23"/>
+        <v>3.4594635926543447</v>
       </c>
       <c r="OD17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.4383235175031039</v>
+        <f t="shared" si="23"/>
+        <v>3.424868956727801</v>
       </c>
       <c r="OE17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.4039402823280729</v>
+        <f t="shared" si="23"/>
+        <v>3.3906202671605228</v>
       </c>
       <c r="OF17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.369900879504792</v>
+        <f t="shared" si="23"/>
+        <v>3.3567140644889175</v>
       </c>
       <c r="OG17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.3362018707097438</v>
+        <f t="shared" si="23"/>
+        <v>3.3231469238440283</v>
       </c>
       <c r="OH17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.3028398520026463</v>
+        <f t="shared" si="23"/>
+        <v>3.289915454605588</v>
       </c>
       <c r="OI17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.2698114534826197</v>
+        <f t="shared" si="23"/>
+        <v>3.257016300059532</v>
       </c>
       <c r="OJ17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.2371133389477933</v>
+        <f t="shared" si="23"/>
+        <v>3.2244461370589366</v>
       </c>
       <c r="OK17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.2047422055583152</v>
+        <f t="shared" si="23"/>
+        <v>3.1922016756883473</v>
       </c>
       <c r="OL17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.1726947835027319</v>
+        <f t="shared" si="23"/>
+        <v>3.1602796589314637</v>
       </c>
       <c r="OM17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.1409678356677047</v>
+        <f t="shared" si="23"/>
+        <v>3.1286768623421488</v>
       </c>
       <c r="ON17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.1095581573110276</v>
+        <f t="shared" si="23"/>
+        <v>3.0973900937187273</v>
       </c>
       <c r="OO17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.0784625757379174</v>
+        <f t="shared" si="23"/>
+        <v>3.0664161927815399</v>
       </c>
       <c r="OP17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.047677949980538</v>
+        <f t="shared" si="23"/>
+        <v>3.0357520308537245</v>
       </c>
       <c r="OQ17" s="5">
-        <f t="shared" si="19"/>
-        <v>3.0172011704807327</v>
+        <f t="shared" si="23"/>
+        <v>3.0053945105451874</v>
       </c>
       <c r="OR17" s="5">
-        <f t="shared" si="19"/>
-        <v>2.9870291587759255</v>
+        <f t="shared" si="23"/>
+        <v>2.9753405654397356</v>
       </c>
       <c r="OS17" s="5">
-        <f t="shared" si="19"/>
-        <v>2.9571588671881663</v>
+        <f t="shared" si="23"/>
+        <v>2.945587159785338</v>
       </c>
       <c r="OT17" s="5">
-        <f t="shared" si="19"/>
-        <v>2.9275872785162846</v>
+        <f t="shared" si="23"/>
+        <v>2.9161312881874846</v>
       </c>
       <c r="OU17" s="5">
-        <f t="shared" si="19"/>
-        <v>2.8983114057311217</v>
+        <f t="shared" si="23"/>
+        <v>2.8869699753056097</v>
       </c>
       <c r="OV17" s="5">
-        <f t="shared" si="19"/>
-        <v>2.8693282916738103</v>
+        <f t="shared" si="23"/>
+        <v>2.8581002755525535</v>
       </c>
       <c r="OW17" s="5">
-        <f t="shared" si="19"/>
-        <v>2.8406350087570722</v>
+        <f t="shared" si="23"/>
+        <v>2.829519272797028</v>
       </c>
       <c r="OX17" s="5">
-        <f t="shared" si="19"/>
-        <v>2.8122286586695013</v>
+        <f t="shared" si="23"/>
+        <v>2.8012240800690575</v>
       </c>
     </row>
-    <row r="18" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:414" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -6463,83 +6475,86 @@
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
     </row>
-    <row r="19" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" ref="C19:T19" si="20">C17/C20</f>
+        <f t="shared" ref="C19:T19" si="24">C17/C20</f>
         <v>0.28699999999999964</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-9.6039603960395695E-2</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.20396039603960392</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-0.36138613861386087</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-0.35490196078431324</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.5886922320550636</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.86176470588235221</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.23970588235294069</v>
       </c>
       <c r="K19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-0.34215686274509693</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.78787878787878862</v>
       </c>
       <c r="M19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.57992202729044973</v>
       </c>
       <c r="N19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.91085271317829264</v>
       </c>
       <c r="O19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.56509161041465816</v>
       </c>
       <c r="P19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.6504854368932038</v>
       </c>
       <c r="Q19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.8723404255319136</v>
       </c>
       <c r="R19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.6352380952380945</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.6928282733339599</v>
       </c>
       <c r="T19" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>2.2530312999342059</v>
       </c>
-      <c r="U19" s="5"/>
+      <c r="U19" s="5">
+        <f t="shared" ref="U19" si="25">U17/U20</f>
+        <v>2.0819625904690282</v>
+      </c>
       <c r="V19" s="5"/>
       <c r="X19" s="5">
         <f>X17/X20</f>
@@ -6559,7 +6574,7 @@
       </c>
       <c r="AB19" s="5">
         <f>AB17/AB20</f>
-        <v>8.0997428571428571</v>
+        <v>8.0680476190476185</v>
       </c>
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
@@ -6572,7 +6587,7 @@
       <c r="AK19" s="5"/>
       <c r="AL19" s="5"/>
     </row>
-    <row r="20" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -6630,7 +6645,9 @@
       <c r="T20" s="5">
         <v>10.638999999999999</v>
       </c>
-      <c r="U20" s="5"/>
+      <c r="U20" s="5">
+        <v>10.638999999999999</v>
+      </c>
       <c r="X20" s="5">
         <f>F20</f>
         <v>10.1</v>
@@ -6661,7 +6678,7 @@
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
     </row>
-    <row r="22" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>46</v>
       </c>
@@ -6670,136 +6687,139 @@
         <v>0.24517466900622106</v>
       </c>
       <c r="D22" s="8">
-        <f t="shared" ref="D22:S22" si="21">D9/D7</f>
+        <f t="shared" ref="D22:S22" si="26">D9/D7</f>
         <v>0.21042304371713369</v>
       </c>
       <c r="E22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.22985458343375914</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.21143154968728287</v>
       </c>
       <c r="G22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.24158492017695715</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.26219361228026733</v>
       </c>
       <c r="I22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.26941923046027788</v>
       </c>
       <c r="J22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.2529923361749763</v>
       </c>
       <c r="K22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.21934026208766388</v>
       </c>
       <c r="L22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.24657632982557307</v>
       </c>
       <c r="M22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.24476047904191625</v>
       </c>
       <c r="N22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.26688867745004746</v>
       </c>
       <c r="O22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.24957940165313439</v>
       </c>
       <c r="P22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.2664595180864161</v>
       </c>
       <c r="Q22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.28993416980813586</v>
       </c>
       <c r="R22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.31034278959810874</v>
       </c>
       <c r="S22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.31136126262040148</v>
       </c>
       <c r="T22" s="8">
-        <f t="shared" ref="T22" si="22">T9/T7</f>
+        <f t="shared" ref="T22:U22" si="27">T9/T7</f>
         <v>0.32902767079457257</v>
       </c>
-      <c r="U22" s="8"/>
+      <c r="U22" s="8">
+        <f t="shared" si="27"/>
+        <v>0.34906017408855805</v>
+      </c>
       <c r="X22" s="8">
-        <f t="shared" ref="X22:AA22" si="23">X9/X7</f>
+        <f t="shared" ref="X22:AA22" si="28">X9/X7</f>
         <v>0.22442016328851699</v>
       </c>
       <c r="Y22" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.25722996328660069</v>
       </c>
       <c r="Z22" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.24603948554711222</v>
       </c>
       <c r="AA22" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.28065911557450973</v>
       </c>
       <c r="AB22" s="8">
-        <f t="shared" ref="AB22:AL22" si="24">AB9/AB7</f>
+        <f t="shared" ref="AB22:AL22" si="29">AB9/AB7</f>
         <v>0.33</v>
       </c>
       <c r="AC22" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.33</v>
       </c>
       <c r="AD22" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.33</v>
       </c>
       <c r="AE22" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.33</v>
       </c>
       <c r="AF22" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.33</v>
       </c>
       <c r="AG22" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.33</v>
       </c>
       <c r="AH22" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.33</v>
       </c>
       <c r="AI22" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="AJ22" s="8">
+        <f t="shared" si="29"/>
+        <v>0.33000000000000007</v>
+      </c>
+      <c r="AK22" s="8">
+        <f t="shared" si="29"/>
         <v>0.33</v>
       </c>
-      <c r="AJ22" s="8">
-        <f t="shared" si="24"/>
+      <c r="AL22" s="8">
+        <f t="shared" si="29"/>
         <v>0.33</v>
       </c>
-      <c r="AK22" s="8">
-        <f t="shared" si="24"/>
-        <v>0.33</v>
-      </c>
-      <c r="AL22" s="8">
-        <f t="shared" si="24"/>
-        <v>0.33000000000000007</v>
-      </c>
     </row>
-    <row r="23" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>47</v>
       </c>
@@ -6808,136 +6828,139 @@
         <v>3.4614771095868531E-2</v>
       </c>
       <c r="D23" s="8">
-        <f t="shared" ref="D23:S23" si="25">D13/D7</f>
+        <f t="shared" ref="D23:S23" si="30">D13/D7</f>
         <v>5.8865081233812379E-3</v>
       </c>
       <c r="E23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>3.1734554511127173E-2</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-1.6851980542043034E-2</v>
       </c>
       <c r="G23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-2.8755529909597951E-2</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>6.3216967896343956E-2</v>
       </c>
       <c r="I23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>7.1893324765041303E-2</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>3.5434426935331054E-2</v>
       </c>
       <c r="K23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-1.5363759602349649E-2</v>
       </c>
       <c r="L23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>4.9949545913219019E-2</v>
       </c>
       <c r="M23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>6.042460533478506E-2</v>
       </c>
       <c r="N23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>8.0399619410085513E-2</v>
       </c>
       <c r="O23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>5.9249506254114584E-2</v>
       </c>
       <c r="P23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>9.8669168083484721E-2</v>
       </c>
       <c r="Q23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.13751195633826585</v>
       </c>
       <c r="R23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.12730496453900705</v>
       </c>
       <c r="S23" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.13432749216664733</v>
       </c>
       <c r="T23" s="8">
-        <f t="shared" ref="T23" si="26">T13/T7</f>
+        <f t="shared" ref="T23:U23" si="31">T13/T7</f>
         <v>0.14457545772352914</v>
       </c>
-      <c r="U23" s="8"/>
+      <c r="U23" s="8">
+        <f t="shared" si="31"/>
+        <v>0.16620411252680706</v>
+      </c>
       <c r="X23" s="8">
-        <f t="shared" ref="X23:AA23" si="27">X13/X7</f>
+        <f t="shared" ref="X23:AA23" si="32">X13/X7</f>
         <v>1.4419757098176195E-2</v>
       </c>
       <c r="Y23" s="8">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>3.8076733151555492E-2</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>4.7728569062908288E-2</v>
       </c>
       <c r="AA23" s="8">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0.10839027223674354</v>
       </c>
       <c r="AB23" s="8">
-        <f t="shared" ref="AB23:AL23" si="28">AB13/AB7</f>
+        <f t="shared" ref="AB23:AL23" si="33">AB13/AB7</f>
         <v>0</v>
       </c>
       <c r="AC23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AD23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AE23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AF23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AG23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AH23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AI23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AJ23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AK23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AL23" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>48</v>
       </c>
@@ -6946,136 +6969,139 @@
         <v>2.2890413144042086E-2</v>
       </c>
       <c r="D24" s="8">
-        <f t="shared" ref="D24:S24" si="29">D17/D7</f>
+        <f t="shared" ref="D24:S24" si="34">D17/D7</f>
         <v>-7.6132171729063371E-3</v>
       </c>
       <c r="E24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>1.6550172732385311E-2</v>
       </c>
       <c r="F24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>-3.1706045865184107E-2</v>
       </c>
       <c r="G24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>-3.4814387382188831E-2</v>
       </c>
       <c r="H24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>4.9409919947181614E-2</v>
       </c>
       <c r="I24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>7.0608080970359005E-2</v>
       </c>
       <c r="J24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>2.1053991216739818E-2</v>
       </c>
       <c r="K24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>-3.1540894713059091E-2</v>
       </c>
       <c r="L24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>5.8094277065013744E-2</v>
       </c>
       <c r="M24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>4.0487207403375157E-2</v>
       </c>
       <c r="N24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>6.3884735625934358E-2</v>
       </c>
       <c r="O24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>4.2864457611001425E-2</v>
       </c>
       <c r="P24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>9.9665826346954339E-2</v>
       </c>
       <c r="Q24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.108929274742587</v>
       </c>
       <c r="R24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.10147754137115834</v>
       </c>
       <c r="S24" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.10450272716722755</v>
       </c>
       <c r="T24" s="8">
-        <f t="shared" ref="T24" si="30">T17/T7</f>
+        <f t="shared" ref="T24:U24" si="35">T17/T7</f>
         <v>0.14202761154233581</v>
       </c>
-      <c r="U24" s="8"/>
+      <c r="U24" s="8">
+        <f t="shared" si="35"/>
+        <v>0.13971237542576001</v>
+      </c>
       <c r="X24" s="8">
-        <f t="shared" ref="X24:AA24" si="31">X17/X7</f>
+        <f t="shared" ref="X24:AA24" si="36">X17/X7</f>
         <v>6.2959502823021617E-4</v>
       </c>
       <c r="Y24" s="8">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>2.9203254825342979E-2</v>
       </c>
       <c r="Z24" s="8">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>3.665200831662041E-2</v>
       </c>
       <c r="AA24" s="8">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>9.3471515262683241E-2</v>
       </c>
       <c r="AB24" s="8">
-        <f t="shared" ref="AB24:AL24" si="32">AB17/AB7</f>
+        <f t="shared" ref="AB24:AL24" si="37">AB17/AB7</f>
         <v>0.13</v>
       </c>
       <c r="AC24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AD24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AE24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AF24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AG24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AH24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AI24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AJ24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AK24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="AL24" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>49</v>
       </c>
@@ -7084,64 +7110,67 @@
         <v>-0.17068112936672508</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" ref="H26:T26" si="33">H7/D7-1</f>
+        <f t="shared" ref="H26:U26" si="38">H7/D7-1</f>
         <v>-4.897574758653167E-2</v>
       </c>
       <c r="I26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>1.6068128866386644E-4</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>8.7734537873522811E-3</v>
       </c>
       <c r="K26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>6.4146951336795599E-2</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0.14500288850375509</v>
       </c>
       <c r="M26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0.18049642541569622</v>
       </c>
       <c r="N26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0.2670283303194696</v>
       </c>
       <c r="O26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0.23551739719837328</v>
       </c>
       <c r="P26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0.22942194032002283</v>
       </c>
       <c r="Q26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0.20937670114316798</v>
       </c>
       <c r="R26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0.14992524126682083</v>
       </c>
       <c r="S26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>0.26062467997951866</v>
       </c>
       <c r="T26" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>-1.0552852201442087E-2</v>
       </c>
-      <c r="U26" s="8"/>
+      <c r="U26" s="8">
+        <f t="shared" si="38"/>
+        <v>-0.10797276768131436</v>
+      </c>
       <c r="Y26" s="8">
-        <f t="shared" ref="Y26:Z26" si="34">Y7/X7-1</f>
+        <f t="shared" ref="Y26:Z26" si="39">Y7/X7-1</f>
         <v>-5.4043624842601279E-2</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>0.16686347338815311</v>
       </c>
       <c r="AA26" s="8">
@@ -7149,51 +7178,51 @@
         <v>0.20372039963936794</v>
       </c>
       <c r="AB26" s="8">
-        <f t="shared" ref="AB26:AL26" si="35">AB7/AA7-1</f>
-        <v>0</v>
+        <f t="shared" ref="AB26:AL26" si="40">AB7/AA7-1</f>
+        <v>-3.9131165833601322E-3</v>
       </c>
       <c r="AC26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AD26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AE26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AF26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AG26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AH26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AI26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AJ26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AK26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AL26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>3.0000000000000027E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:414" x14ac:dyDescent="0.2">
       <c r="AP29" t="s">
         <v>50</v>
       </c>
@@ -7201,7 +7230,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -7210,64 +7239,64 @@
         <v>-0.15420560747663536</v>
       </c>
       <c r="G30" s="8">
-        <f t="shared" ref="G30:S32" si="36">G2/D2-1</f>
+        <f t="shared" ref="G30:S32" si="41">G2/D2-1</f>
         <v>-0.17727272727272725</v>
       </c>
       <c r="H30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.11910669975186106</v>
       </c>
       <c r="I30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.32044198895027609</v>
       </c>
       <c r="J30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.44751381215469599</v>
       </c>
       <c r="K30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-3.3259423503325891E-2</v>
       </c>
       <c r="L30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.15899581589958167</v>
       </c>
       <c r="M30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.1507633587786259</v>
       </c>
       <c r="N30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.34633027522935778</v>
       </c>
       <c r="O30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>6.1371841155234641E-2</v>
       </c>
       <c r="P30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.17744610281923712</v>
       </c>
       <c r="Q30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.30153321976149927</v>
       </c>
       <c r="R30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.3962585034013606</v>
       </c>
       <c r="S30" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.17183098591549295</v>
       </c>
       <c r="T30" s="8">
-        <f t="shared" ref="T30:U32" si="37">T2/Q2-1</f>
+        <f t="shared" ref="T30:U32" si="42">T2/Q2-1</f>
         <v>0.14005235602094235</v>
       </c>
       <c r="U30" s="8">
-        <f t="shared" si="37"/>
-        <v>-4.5188794153471323E-2</v>
+        <f t="shared" si="42"/>
+        <v>-8.8915956151035314E-2</v>
       </c>
       <c r="AP30" t="s">
         <v>51</v>
@@ -7276,180 +7305,180 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="31" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>60</v>
       </c>
       <c r="F31" s="8">
-        <f t="shared" ref="F31:F32" si="38">F3/C3-1</f>
+        <f t="shared" ref="F31:F32" si="43">F3/C3-1</f>
         <v>-7.6576576576576572E-2</v>
       </c>
       <c r="G31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-7.999999999999996E-2</v>
       </c>
       <c r="H31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.12584269662921355</v>
       </c>
       <c r="I31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-6.0975609756097615E-2</v>
       </c>
       <c r="J31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.12531969309462909</v>
       </c>
       <c r="K31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-2.0565552699228773E-2</v>
       </c>
       <c r="L31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.11688311688311681</v>
       </c>
       <c r="M31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.17836257309941494</v>
       </c>
       <c r="N31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.14435695538057747</v>
       </c>
       <c r="O31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>1.6279069767441978E-2</v>
       </c>
       <c r="P31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.14392059553349879</v>
       </c>
       <c r="Q31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.153669724770642</v>
       </c>
       <c r="R31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>7.5514874141876298E-2</v>
       </c>
       <c r="S31" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.15835140997830788</v>
       </c>
       <c r="T31" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>8.9463220675944255E-2</v>
       </c>
       <c r="U31" s="8">
-        <f t="shared" si="37"/>
-        <v>0.16595744680851054</v>
+        <f t="shared" si="42"/>
+        <v>0.10000000000000009</v>
       </c>
       <c r="AP31" t="s">
         <v>52</v>
       </c>
       <c r="AQ31" s="12">
         <f>NPV(AQ29,AB17:OX17)</f>
-        <v>1242.4647992513835</v>
+        <v>1237.6028896411899</v>
       </c>
     </row>
-    <row r="32" spans="2:414" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:414" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>61</v>
       </c>
       <c r="F32" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="43"/>
         <v>-1.0443864229764954E-2</v>
       </c>
       <c r="G32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.29828850855745725</v>
       </c>
       <c r="H32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-6.2972292191435741E-2</v>
       </c>
       <c r="I32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>7.9155672823221224E-3</v>
       </c>
       <c r="J32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>2.7874564459930307E-2</v>
       </c>
       <c r="K32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.22311827956989261</v>
       </c>
       <c r="L32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>5.4973821989528604E-2</v>
       </c>
       <c r="M32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.56949152542372872</v>
       </c>
       <c r="N32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.55017301038062283</v>
       </c>
       <c r="O32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.15136476426798995</v>
       </c>
       <c r="P32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.15550755939524841</v>
       </c>
       <c r="Q32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.140625</v>
       </c>
       <c r="R32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.17251461988304095</v>
       </c>
       <c r="S32" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.33084112149532718</v>
       </c>
       <c r="T32" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>-0.47553816046966735</v>
       </c>
       <c r="U32" s="8">
-        <f t="shared" si="37"/>
-        <v>-0.29825436408977557</v>
+        <f t="shared" si="42"/>
+        <v>-0.20099750623441404</v>
       </c>
       <c r="AP32" t="s">
         <v>53</v>
       </c>
       <c r="AQ32" s="13">
         <f>AQ31/Main!K2</f>
-        <v>116.86087276630771</v>
+        <v>116.40358254713976</v>
       </c>
     </row>
-    <row r="33" spans="32:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="32:45" x14ac:dyDescent="0.2">
       <c r="AP33" t="s">
         <v>54</v>
       </c>
       <c r="AQ33" s="8">
         <f>AQ32/Main!K1-1</f>
-        <v>1.2216895963176371</v>
+        <v>0.57493684950804713</v>
       </c>
     </row>
-    <row r="35" spans="32:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="32:45" x14ac:dyDescent="0.2">
       <c r="AR35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS35" s="15">
         <f>(AQ32*500)-(500*49.51)</f>
-        <v>33675.43638315385</v>
+        <v>33446.791273569885</v>
       </c>
     </row>
-    <row r="37" spans="32:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="32:45" x14ac:dyDescent="0.2">
       <c r="AF37">
         <f>52/AB19</f>
-        <v>6.4199568945751366</v>
+        <v>6.4451776260262417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>